<commit_message>
forecast updates and automation
</commit_message>
<xml_diff>
--- a/outputs/aht/fs_res_aht_monthly.xlsx
+++ b/outputs/aht/fs_res_aht_monthly.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,40 +524,40 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>42736</v>
+        <v>42887</v>
       </c>
       <c r="C2" t="n">
-        <v>366.2813661570577</v>
+        <v>393.551468132402</v>
       </c>
       <c r="D2" t="n">
-        <v>348.2761607531469</v>
+        <v>359.5883839977516</v>
       </c>
       <c r="E2" t="n">
-        <v>392.5595282214107</v>
+        <v>404.4588205188832</v>
       </c>
       <c r="F2" t="n">
-        <v>366.2813661570577</v>
+        <v>393.551468132402</v>
       </c>
       <c r="G2" t="n">
-        <v>366.2813661570577</v>
+        <v>393.551468132402</v>
       </c>
       <c r="H2" t="n">
-        <v>3.015601448873467</v>
+        <v>-10.80953905594185</v>
       </c>
       <c r="I2" t="n">
-        <v>3.015601448873467</v>
+        <v>-10.80953905594185</v>
       </c>
       <c r="J2" t="n">
-        <v>3.015601448873467</v>
+        <v>-10.80953905594185</v>
       </c>
       <c r="K2" t="n">
-        <v>3.015601448873467</v>
+        <v>-10.80953905594185</v>
       </c>
       <c r="L2" t="n">
-        <v>3.015601448873467</v>
+        <v>-10.80953905594185</v>
       </c>
       <c r="M2" t="n">
-        <v>3.015601448873467</v>
+        <v>-10.80953905594185</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -569,7 +569,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>369.2969676059312</v>
+        <v>382.7419290764601</v>
       </c>
     </row>
     <row r="3">
@@ -577,40 +577,40 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>42767</v>
+        <v>42917</v>
       </c>
       <c r="C3" t="n">
-        <v>369.0094303020272</v>
+        <v>395.2744167334855</v>
       </c>
       <c r="D3" t="n">
-        <v>337.4758198738668</v>
+        <v>361.9982293498173</v>
       </c>
       <c r="E3" t="n">
-        <v>381.1073869675101</v>
+        <v>408.0444068336275</v>
       </c>
       <c r="F3" t="n">
-        <v>369.0094303020272</v>
+        <v>395.2744167334855</v>
       </c>
       <c r="G3" t="n">
-        <v>369.0094303020272</v>
+        <v>395.2744167334855</v>
       </c>
       <c r="H3" t="n">
-        <v>-10.44845217156965</v>
+        <v>-8.794431777412505</v>
       </c>
       <c r="I3" t="n">
-        <v>-10.44845217156965</v>
+        <v>-8.794431777412505</v>
       </c>
       <c r="J3" t="n">
-        <v>-10.44845217156965</v>
+        <v>-8.794431777412505</v>
       </c>
       <c r="K3" t="n">
-        <v>-10.44845217156965</v>
+        <v>-8.794431777412505</v>
       </c>
       <c r="L3" t="n">
-        <v>-10.44845217156965</v>
+        <v>-8.794431777412505</v>
       </c>
       <c r="M3" t="n">
-        <v>-10.44845217156965</v>
+        <v>-8.794431777412505</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -622,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>358.5609781304575</v>
+        <v>386.4799849560729</v>
       </c>
     </row>
     <row r="4">
@@ -630,40 +630,40 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>42795</v>
+        <v>42948</v>
       </c>
       <c r="C4" t="n">
-        <v>371.473488239419</v>
+        <v>397.054796954605</v>
       </c>
       <c r="D4" t="n">
-        <v>335.3326152791469</v>
+        <v>358.8898837802088</v>
       </c>
       <c r="E4" t="n">
-        <v>379.2132603621647</v>
+        <v>405.1282174575452</v>
       </c>
       <c r="F4" t="n">
-        <v>371.473488239419</v>
+        <v>397.054796954605</v>
       </c>
       <c r="G4" t="n">
-        <v>371.473488239419</v>
+        <v>397.054796954605</v>
       </c>
       <c r="H4" t="n">
-        <v>-14.10656901540339</v>
+        <v>-14.36160343907189</v>
       </c>
       <c r="I4" t="n">
-        <v>-14.10656901540339</v>
+        <v>-14.36160343907189</v>
       </c>
       <c r="J4" t="n">
-        <v>-14.10656901540339</v>
+        <v>-14.36160343907189</v>
       </c>
       <c r="K4" t="n">
-        <v>-14.10656901540339</v>
+        <v>-14.36160343907189</v>
       </c>
       <c r="L4" t="n">
-        <v>-14.10656901540339</v>
+        <v>-14.36160343907189</v>
       </c>
       <c r="M4" t="n">
-        <v>-14.10656901540339</v>
+        <v>-14.36160343907189</v>
       </c>
       <c r="N4" t="n">
         <v>0</v>
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>357.3669192240156</v>
+        <v>382.6931935155332</v>
       </c>
     </row>
     <row r="5">
@@ -683,40 +683,40 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>42826</v>
+        <v>42979</v>
       </c>
       <c r="C5" t="n">
-        <v>374.2015535582671</v>
+        <v>398.8351771687829</v>
       </c>
       <c r="D5" t="n">
-        <v>326.4771715051639</v>
+        <v>366.7894093134217</v>
       </c>
       <c r="E5" t="n">
-        <v>374.8329521442034</v>
+        <v>410.1916060313924</v>
       </c>
       <c r="F5" t="n">
-        <v>374.2015535582671</v>
+        <v>398.8351771687829</v>
       </c>
       <c r="G5" t="n">
-        <v>374.2015535582671</v>
+        <v>398.8351771687829</v>
       </c>
       <c r="H5" t="n">
-        <v>-23.39617043646516</v>
+        <v>-10.25289263084141</v>
       </c>
       <c r="I5" t="n">
-        <v>-23.39617043646516</v>
+        <v>-10.25289263084141</v>
       </c>
       <c r="J5" t="n">
-        <v>-23.39617043646516</v>
+        <v>-10.25289263084141</v>
       </c>
       <c r="K5" t="n">
-        <v>-23.39617043646516</v>
+        <v>-10.25289263084141</v>
       </c>
       <c r="L5" t="n">
-        <v>-23.39617043646516</v>
+        <v>-10.25289263084141</v>
       </c>
       <c r="M5" t="n">
-        <v>-23.39617043646516</v>
+        <v>-10.25289263084141</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>350.8053831218019</v>
+        <v>388.5822845379415</v>
       </c>
     </row>
     <row r="6">
@@ -736,40 +736,40 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>42856</v>
+        <v>43009</v>
       </c>
       <c r="C6" t="n">
-        <v>376.8416167700556</v>
+        <v>400.5581257631486</v>
       </c>
       <c r="D6" t="n">
-        <v>348.2529945553987</v>
+        <v>376.9818360127215</v>
       </c>
       <c r="E6" t="n">
-        <v>393.6090536655371</v>
+        <v>419.5122408261207</v>
       </c>
       <c r="F6" t="n">
-        <v>376.8416167700556</v>
+        <v>400.5581257631486</v>
       </c>
       <c r="G6" t="n">
-        <v>376.8416167700556</v>
+        <v>400.5581257631486</v>
       </c>
       <c r="H6" t="n">
-        <v>-6.776698958476485</v>
+        <v>-3.024207560303538</v>
       </c>
       <c r="I6" t="n">
-        <v>-6.776698958476485</v>
+        <v>-3.024207560303538</v>
       </c>
       <c r="J6" t="n">
-        <v>-6.776698958476485</v>
+        <v>-3.024207560303538</v>
       </c>
       <c r="K6" t="n">
-        <v>-6.776698958476485</v>
+        <v>-3.024207560303538</v>
       </c>
       <c r="L6" t="n">
-        <v>-6.776698958476485</v>
+        <v>-3.024207560303538</v>
       </c>
       <c r="M6" t="n">
-        <v>-6.776698958476485</v>
+        <v>-3.024207560303538</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -781,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>370.0649178115791</v>
+        <v>397.5339182028451</v>
       </c>
     </row>
     <row r="7">
@@ -789,40 +789,40 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>42887</v>
+        <v>43040</v>
       </c>
       <c r="C7" t="n">
-        <v>379.569682217446</v>
+        <v>402.3385059904093</v>
       </c>
       <c r="D7" t="n">
-        <v>343.275554912427</v>
+        <v>392.3201976318019</v>
       </c>
       <c r="E7" t="n">
-        <v>388.0194763888708</v>
+        <v>436.9661307618012</v>
       </c>
       <c r="F7" t="n">
-        <v>379.569682217446</v>
+        <v>402.3385059904093</v>
       </c>
       <c r="G7" t="n">
-        <v>379.569682217446</v>
+        <v>402.3385059904093</v>
       </c>
       <c r="H7" t="n">
-        <v>-14.76870261917891</v>
+        <v>12.30749244748804</v>
       </c>
       <c r="I7" t="n">
-        <v>-14.76870261917891</v>
+        <v>12.30749244748804</v>
       </c>
       <c r="J7" t="n">
-        <v>-14.76870261917891</v>
+        <v>12.30749244748804</v>
       </c>
       <c r="K7" t="n">
-        <v>-14.76870261917891</v>
+        <v>12.30749244748804</v>
       </c>
       <c r="L7" t="n">
-        <v>-14.76870261917891</v>
+        <v>12.30749244748804</v>
       </c>
       <c r="M7" t="n">
-        <v>-14.76870261917891</v>
+        <v>12.30749244748804</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>364.8009795982671</v>
+        <v>414.6459984378973</v>
       </c>
     </row>
     <row r="8">
@@ -842,40 +842,40 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>42917</v>
+        <v>43070</v>
       </c>
       <c r="C8" t="n">
-        <v>382.2097455536304</v>
+        <v>404.0614545974358</v>
       </c>
       <c r="D8" t="n">
-        <v>349.9639501434391</v>
+        <v>401.5936112514897</v>
       </c>
       <c r="E8" t="n">
-        <v>394.5729465602923</v>
+        <v>446.4253402595234</v>
       </c>
       <c r="F8" t="n">
-        <v>382.2097455536304</v>
+        <v>404.0614545974358</v>
       </c>
       <c r="G8" t="n">
-        <v>382.2097455536304</v>
+        <v>404.0614545974358</v>
       </c>
       <c r="H8" t="n">
-        <v>-8.508871626378498</v>
+        <v>20.18722681309875</v>
       </c>
       <c r="I8" t="n">
-        <v>-8.508871626378498</v>
+        <v>20.18722681309875</v>
       </c>
       <c r="J8" t="n">
-        <v>-8.508871626378498</v>
+        <v>20.18722681309875</v>
       </c>
       <c r="K8" t="n">
-        <v>-8.508871626378498</v>
+        <v>20.18722681309875</v>
       </c>
       <c r="L8" t="n">
-        <v>-8.508871626378498</v>
+        <v>20.18722681309875</v>
       </c>
       <c r="M8" t="n">
-        <v>-8.508871626378498</v>
+        <v>20.18722681309875</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>373.7008739272519</v>
+        <v>424.2486814105346</v>
       </c>
     </row>
     <row r="9">
@@ -895,40 +895,40 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>42948</v>
+        <v>43101</v>
       </c>
       <c r="C9" t="n">
-        <v>384.9378104376204</v>
+        <v>405.8418412140693</v>
       </c>
       <c r="D9" t="n">
-        <v>348.0054035493063</v>
+        <v>401.0958321029538</v>
       </c>
       <c r="E9" t="n">
-        <v>394.4155436309626</v>
+        <v>443.3252127518767</v>
       </c>
       <c r="F9" t="n">
-        <v>384.9378104376204</v>
+        <v>405.8418412140693</v>
       </c>
       <c r="G9" t="n">
-        <v>384.9378104376204</v>
+        <v>405.8418412140693</v>
       </c>
       <c r="H9" t="n">
-        <v>-14.97240095259227</v>
+        <v>16.85658590101929</v>
       </c>
       <c r="I9" t="n">
-        <v>-14.97240095259227</v>
+        <v>16.85658590101929</v>
       </c>
       <c r="J9" t="n">
-        <v>-14.97240095259227</v>
+        <v>16.85658590101929</v>
       </c>
       <c r="K9" t="n">
-        <v>-14.97240095259227</v>
+        <v>16.85658590101929</v>
       </c>
       <c r="L9" t="n">
-        <v>-14.97240095259227</v>
+        <v>16.85658590101929</v>
       </c>
       <c r="M9" t="n">
-        <v>-14.97240095259227</v>
+        <v>16.85658590101929</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
@@ -940,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>369.9654094850281</v>
+        <v>422.6984271150886</v>
       </c>
     </row>
     <row r="10">
@@ -948,40 +948,40 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>42979</v>
+        <v>43132</v>
       </c>
       <c r="C10" t="n">
-        <v>387.6658753216104</v>
+        <v>407.6222278307029</v>
       </c>
       <c r="D10" t="n">
-        <v>352.6685128386545</v>
+        <v>381.4133408434552</v>
       </c>
       <c r="E10" t="n">
-        <v>397.0147915816039</v>
+        <v>424.7149076757688</v>
       </c>
       <c r="F10" t="n">
-        <v>387.6658753216104</v>
+        <v>407.6222278307029</v>
       </c>
       <c r="G10" t="n">
-        <v>387.6658753216104</v>
+        <v>407.6222278307029</v>
       </c>
       <c r="H10" t="n">
-        <v>-13.19604518690804</v>
+        <v>-4.658038359042022</v>
       </c>
       <c r="I10" t="n">
-        <v>-13.19604518690804</v>
+        <v>-4.658038359042022</v>
       </c>
       <c r="J10" t="n">
-        <v>-13.19604518690804</v>
+        <v>-4.658038359042022</v>
       </c>
       <c r="K10" t="n">
-        <v>-13.19604518690804</v>
+        <v>-4.658038359042022</v>
       </c>
       <c r="L10" t="n">
-        <v>-13.19604518690804</v>
+        <v>-4.658038359042022</v>
       </c>
       <c r="M10" t="n">
-        <v>-13.19604518690804</v>
+        <v>-4.658038359042022</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -993,7 +993,7 @@
         <v>0</v>
       </c>
       <c r="Q10" t="n">
-        <v>374.4698301347023</v>
+        <v>402.9641894716609</v>
       </c>
     </row>
     <row r="11">
@@ -1001,40 +1001,40 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>43009</v>
+        <v>43160</v>
       </c>
       <c r="C11" t="n">
-        <v>390.3058395223918</v>
+        <v>409.2303189787826</v>
       </c>
       <c r="D11" t="n">
-        <v>365.3737765694258</v>
+        <v>360.2001772025565</v>
       </c>
       <c r="E11" t="n">
-        <v>408.2246682632477</v>
+        <v>402.9642684750812</v>
       </c>
       <c r="F11" t="n">
-        <v>390.3058395223918</v>
+        <v>409.2303189787826</v>
       </c>
       <c r="G11" t="n">
-        <v>390.3058395223918</v>
+        <v>409.2303189787826</v>
       </c>
       <c r="H11" t="n">
-        <v>-2.977234654771979</v>
+        <v>-27.6690229730164</v>
       </c>
       <c r="I11" t="n">
-        <v>-2.977234654771979</v>
+        <v>-27.6690229730164</v>
       </c>
       <c r="J11" t="n">
-        <v>-2.977234654771979</v>
+        <v>-27.6690229730164</v>
       </c>
       <c r="K11" t="n">
-        <v>-2.977234654771979</v>
+        <v>-27.6690229730164</v>
       </c>
       <c r="L11" t="n">
-        <v>-2.977234654771979</v>
+        <v>-27.6690229730164</v>
       </c>
       <c r="M11" t="n">
-        <v>-2.977234654771979</v>
+        <v>-27.6690229730164</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -1046,7 +1046,7 @@
         <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>387.3286048676198</v>
+        <v>381.5612960057662</v>
       </c>
     </row>
     <row r="12">
@@ -1054,40 +1054,40 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>43040</v>
+        <v>43191</v>
       </c>
       <c r="C12" t="n">
-        <v>393.033802529866</v>
+        <v>411.0107056134757</v>
       </c>
       <c r="D12" t="n">
-        <v>385.7978361119251</v>
+        <v>374.7782841985727</v>
       </c>
       <c r="E12" t="n">
-        <v>430.1368186507697</v>
+        <v>417.8459834320261</v>
       </c>
       <c r="F12" t="n">
-        <v>393.033802529866</v>
+        <v>411.0107056134757</v>
       </c>
       <c r="G12" t="n">
-        <v>393.033802529866</v>
+        <v>411.0107056134757</v>
       </c>
       <c r="H12" t="n">
-        <v>15.93712598273145</v>
+        <v>-13.69925229559566</v>
       </c>
       <c r="I12" t="n">
-        <v>15.93712598273145</v>
+        <v>-13.69925229559566</v>
       </c>
       <c r="J12" t="n">
-        <v>15.93712598273145</v>
+        <v>-13.69925229559566</v>
       </c>
       <c r="K12" t="n">
-        <v>15.93712598273145</v>
+        <v>-13.69925229559566</v>
       </c>
       <c r="L12" t="n">
-        <v>15.93712598273145</v>
+        <v>-13.69925229559566</v>
       </c>
       <c r="M12" t="n">
-        <v>15.93712598273145</v>
+        <v>-13.69925229559566</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="Q12" t="n">
-        <v>408.9709285125974</v>
+        <v>397.31145331788</v>
       </c>
     </row>
     <row r="13">
@@ -1107,40 +1107,40 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>43070</v>
+        <v>43221</v>
       </c>
       <c r="C13" t="n">
-        <v>395.6730985143476</v>
+        <v>412.7336604212432</v>
       </c>
       <c r="D13" t="n">
-        <v>396.5548950506995</v>
+        <v>377.5295705282419</v>
       </c>
       <c r="E13" t="n">
-        <v>440.6292453025073</v>
+        <v>424.3863329498732</v>
       </c>
       <c r="F13" t="n">
-        <v>395.6730985143476</v>
+        <v>412.7336604212432</v>
       </c>
       <c r="G13" t="n">
-        <v>395.6730985143476</v>
+        <v>412.7336604212432</v>
       </c>
       <c r="H13" t="n">
-        <v>22.87694430916519</v>
+        <v>-11.47527954759939</v>
       </c>
       <c r="I13" t="n">
-        <v>22.87694430916519</v>
+        <v>-11.47527954759939</v>
       </c>
       <c r="J13" t="n">
-        <v>22.87694430916519</v>
+        <v>-11.47527954759939</v>
       </c>
       <c r="K13" t="n">
-        <v>22.87694430916519</v>
+        <v>-11.47527954759939</v>
       </c>
       <c r="L13" t="n">
-        <v>22.87694430916519</v>
+        <v>-11.47527954759939</v>
       </c>
       <c r="M13" t="n">
-        <v>22.87694430916519</v>
+        <v>-11.47527954759939</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="Q13" t="n">
-        <v>418.5500428235128</v>
+        <v>401.2583808736438</v>
       </c>
     </row>
     <row r="14">
@@ -1160,40 +1160,40 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>43101</v>
+        <v>43252</v>
       </c>
       <c r="C14" t="n">
-        <v>398.4003710316453</v>
+        <v>414.5140470722872</v>
       </c>
       <c r="D14" t="n">
-        <v>386.1779222869479</v>
+        <v>391.5540139031021</v>
       </c>
       <c r="E14" t="n">
-        <v>429.9363671600534</v>
+        <v>433.9340218536217</v>
       </c>
       <c r="F14" t="n">
-        <v>398.4003710316453</v>
+        <v>414.5140470722872</v>
       </c>
       <c r="G14" t="n">
-        <v>398.4003710316453</v>
+        <v>414.5140470722872</v>
       </c>
       <c r="H14" t="n">
-        <v>9.860895339181967</v>
+        <v>-1.964082117542675</v>
       </c>
       <c r="I14" t="n">
-        <v>9.860895339181967</v>
+        <v>-1.964082117542675</v>
       </c>
       <c r="J14" t="n">
-        <v>9.860895339181967</v>
+        <v>-1.964082117542675</v>
       </c>
       <c r="K14" t="n">
-        <v>9.860895339181967</v>
+        <v>-1.964082117542675</v>
       </c>
       <c r="L14" t="n">
-        <v>9.860895339181967</v>
+        <v>-1.964082117542675</v>
       </c>
       <c r="M14" t="n">
-        <v>9.860895339181967</v>
+        <v>-1.964082117542675</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="Q14" t="n">
-        <v>408.2612663708273</v>
+        <v>412.5499649547446</v>
       </c>
     </row>
     <row r="15">
@@ -1213,40 +1213,40 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>43132</v>
+        <v>43282</v>
       </c>
       <c r="C15" t="n">
-        <v>401.1276071815911</v>
+        <v>416.2370018958782</v>
       </c>
       <c r="D15" t="n">
-        <v>367.8800329631735</v>
+        <v>381.9710254118432</v>
       </c>
       <c r="E15" t="n">
-        <v>412.542478179982</v>
+        <v>426.432127121026</v>
       </c>
       <c r="F15" t="n">
-        <v>401.1276071815911</v>
+        <v>416.2370018958782</v>
       </c>
       <c r="G15" t="n">
-        <v>401.1276071815911</v>
+        <v>416.2370018958782</v>
       </c>
       <c r="H15" t="n">
-        <v>-10.17627712678718</v>
+        <v>-13.63613033147186</v>
       </c>
       <c r="I15" t="n">
-        <v>-10.17627712678718</v>
+        <v>-13.63613033147186</v>
       </c>
       <c r="J15" t="n">
-        <v>-10.17627712678718</v>
+        <v>-13.63613033147186</v>
       </c>
       <c r="K15" t="n">
-        <v>-10.17627712678718</v>
+        <v>-13.63613033147186</v>
       </c>
       <c r="L15" t="n">
-        <v>-10.17627712678718</v>
+        <v>-13.63613033147186</v>
       </c>
       <c r="M15" t="n">
-        <v>-10.17627712678718</v>
+        <v>-13.63613033147186</v>
       </c>
       <c r="N15" t="n">
         <v>0</v>
@@ -1258,7 +1258,7 @@
         <v>0</v>
       </c>
       <c r="Q15" t="n">
-        <v>390.9513300548039</v>
+        <v>402.6008715644063</v>
       </c>
     </row>
     <row r="16">
@@ -1266,40 +1266,40 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>43160</v>
+        <v>43313</v>
       </c>
       <c r="C16" t="n">
-        <v>403.5909172525098</v>
+        <v>418.0173885398815</v>
       </c>
       <c r="D16" t="n">
-        <v>348.5409819265206</v>
+        <v>378.983795665974</v>
       </c>
       <c r="E16" t="n">
-        <v>393.9402526732007</v>
+        <v>423.9567633575043</v>
       </c>
       <c r="F16" t="n">
-        <v>403.5909172525098</v>
+        <v>418.0173885398815</v>
       </c>
       <c r="G16" t="n">
-        <v>403.5909172525098</v>
+        <v>418.0173885398815</v>
       </c>
       <c r="H16" t="n">
-        <v>-33.02313200123849</v>
+        <v>-15.4619285277358</v>
       </c>
       <c r="I16" t="n">
-        <v>-33.02313200123849</v>
+        <v>-15.4619285277358</v>
       </c>
       <c r="J16" t="n">
-        <v>-33.02313200123849</v>
+        <v>-15.4619285277358</v>
       </c>
       <c r="K16" t="n">
-        <v>-33.02313200123849</v>
+        <v>-15.4619285277358</v>
       </c>
       <c r="L16" t="n">
-        <v>-33.02313200123849</v>
+        <v>-15.4619285277358</v>
       </c>
       <c r="M16" t="n">
-        <v>-33.02313200123849</v>
+        <v>-15.4619285277358</v>
       </c>
       <c r="N16" t="n">
         <v>0</v>
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="Q16" t="n">
-        <v>370.5677852512713</v>
+        <v>402.5554600121457</v>
       </c>
     </row>
     <row r="17">
@@ -1319,40 +1319,40 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>43191</v>
+        <v>43344</v>
       </c>
       <c r="C17" t="n">
-        <v>406.3158374454517</v>
+        <v>419.7977751838847</v>
       </c>
       <c r="D17" t="n">
-        <v>368.3510830762124</v>
+        <v>376.5496382092143</v>
       </c>
       <c r="E17" t="n">
-        <v>417.3567772385205</v>
+        <v>421.4937267401392</v>
       </c>
       <c r="F17" t="n">
-        <v>406.3158374454517</v>
+        <v>419.7977751838847</v>
       </c>
       <c r="G17" t="n">
-        <v>406.3158374454517</v>
+        <v>419.7977751838847</v>
       </c>
       <c r="H17" t="n">
-        <v>-13.97176645238149</v>
+        <v>-19.27572644503732</v>
       </c>
       <c r="I17" t="n">
-        <v>-13.97176645238149</v>
+        <v>-19.27572644503732</v>
       </c>
       <c r="J17" t="n">
-        <v>-13.97176645238149</v>
+        <v>-19.27572644503732</v>
       </c>
       <c r="K17" t="n">
-        <v>-13.97176645238149</v>
+        <v>-19.27572644503732</v>
       </c>
       <c r="L17" t="n">
-        <v>-13.97176645238149</v>
+        <v>-19.27572644503732</v>
       </c>
       <c r="M17" t="n">
-        <v>-13.97176645238149</v>
+        <v>-19.27572644503732</v>
       </c>
       <c r="N17" t="n">
         <v>0</v>
@@ -1364,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="Q17" t="n">
-        <v>392.3440709930702</v>
+        <v>400.5220487388474</v>
       </c>
     </row>
     <row r="18">
@@ -1372,40 +1372,40 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>43221</v>
+        <v>43374</v>
       </c>
       <c r="C18" t="n">
-        <v>408.9528569870083</v>
+        <v>421.5207300064721</v>
       </c>
       <c r="D18" t="n">
-        <v>383.9101152775943</v>
+        <v>395.3204564418875</v>
       </c>
       <c r="E18" t="n">
-        <v>428.0170301433971</v>
+        <v>440.2822788918991</v>
       </c>
       <c r="F18" t="n">
-        <v>408.9528569870083</v>
+        <v>421.5207300064721</v>
       </c>
       <c r="G18" t="n">
-        <v>408.9528569870083</v>
+        <v>421.5207300064721</v>
       </c>
       <c r="H18" t="n">
-        <v>-4.207841127828341</v>
+        <v>-3.350966490776475</v>
       </c>
       <c r="I18" t="n">
-        <v>-4.207841127828341</v>
+        <v>-3.350966490776475</v>
       </c>
       <c r="J18" t="n">
-        <v>-4.207841127828341</v>
+        <v>-3.350966490776475</v>
       </c>
       <c r="K18" t="n">
-        <v>-4.207841127828341</v>
+        <v>-3.350966490776475</v>
       </c>
       <c r="L18" t="n">
-        <v>-4.207841127828341</v>
+        <v>-3.350966490776475</v>
       </c>
       <c r="M18" t="n">
-        <v>-4.207841127828341</v>
+        <v>-3.350966490776475</v>
       </c>
       <c r="N18" t="n">
         <v>0</v>
@@ -1417,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="Q18" t="n">
-        <v>404.74501585918</v>
+        <v>418.1697635156956</v>
       </c>
     </row>
     <row r="19">
@@ -1425,40 +1425,40 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>43252</v>
+        <v>43405</v>
       </c>
       <c r="C19" t="n">
-        <v>411.1662827195757</v>
+        <v>423.301116656479</v>
       </c>
       <c r="D19" t="n">
-        <v>385.4382299371495</v>
+        <v>416.0804485730261</v>
       </c>
       <c r="E19" t="n">
-        <v>429.3305350632923</v>
+        <v>460.7482644799497</v>
       </c>
       <c r="F19" t="n">
-        <v>411.1662827195757</v>
+        <v>423.301116656479</v>
       </c>
       <c r="G19" t="n">
-        <v>411.1662827195757</v>
+        <v>423.301116656479</v>
       </c>
       <c r="H19" t="n">
-        <v>-4.849368453395059</v>
+        <v>14.86949953645415</v>
       </c>
       <c r="I19" t="n">
-        <v>-4.849368453395059</v>
+        <v>14.86949953645415</v>
       </c>
       <c r="J19" t="n">
-        <v>-4.849368453395059</v>
+        <v>14.86949953645415</v>
       </c>
       <c r="K19" t="n">
-        <v>-4.849368453395059</v>
+        <v>14.86949953645415</v>
       </c>
       <c r="L19" t="n">
-        <v>-4.849368453395059</v>
+        <v>14.86949953645415</v>
       </c>
       <c r="M19" t="n">
-        <v>-4.849368453395059</v>
+        <v>14.86949953645415</v>
       </c>
       <c r="N19" t="n">
         <v>0</v>
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
       <c r="Q19" t="n">
-        <v>406.3169142661807</v>
+        <v>438.1706161929332</v>
       </c>
     </row>
     <row r="20">
@@ -1478,40 +1478,40 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>43282</v>
+        <v>43435</v>
       </c>
       <c r="C20" t="n">
-        <v>413.3083076220604</v>
+        <v>425.0240714741817</v>
       </c>
       <c r="D20" t="n">
-        <v>375.0319094043103</v>
+        <v>432.7031800160763</v>
       </c>
       <c r="E20" t="n">
-        <v>422.4989369757776</v>
+        <v>475.9575091057432</v>
       </c>
       <c r="F20" t="n">
-        <v>413.3083076220604</v>
+        <v>425.0240714741817</v>
       </c>
       <c r="G20" t="n">
-        <v>413.3083076220604</v>
+        <v>425.0240714741817</v>
       </c>
       <c r="H20" t="n">
-        <v>-14.33122397254093</v>
+        <v>29.31348123824995</v>
       </c>
       <c r="I20" t="n">
-        <v>-14.33122397254093</v>
+        <v>29.31348123824995</v>
       </c>
       <c r="J20" t="n">
-        <v>-14.33122397254093</v>
+        <v>29.31348123824995</v>
       </c>
       <c r="K20" t="n">
-        <v>-14.33122397254093</v>
+        <v>29.31348123824995</v>
       </c>
       <c r="L20" t="n">
-        <v>-14.33122397254093</v>
+        <v>29.31348123824995</v>
       </c>
       <c r="M20" t="n">
-        <v>-14.33122397254093</v>
+        <v>29.31348123824995</v>
       </c>
       <c r="N20" t="n">
         <v>0</v>
@@ -1523,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="Q20" t="n">
-        <v>398.9770836495194</v>
+        <v>454.3375527124316</v>
       </c>
     </row>
     <row r="21">
@@ -1531,40 +1531,40 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>43313</v>
+        <v>43466</v>
       </c>
       <c r="C21" t="n">
-        <v>415.5173956444393</v>
+        <v>426.8044581191411</v>
       </c>
       <c r="D21" t="n">
-        <v>378.5565498650249</v>
+        <v>423.0856493150729</v>
       </c>
       <c r="E21" t="n">
-        <v>422.1897444315583</v>
+        <v>468.9089422376933</v>
       </c>
       <c r="F21" t="n">
-        <v>415.5173956444393</v>
+        <v>426.8044581191411</v>
       </c>
       <c r="G21" t="n">
-        <v>415.5173956444393</v>
+        <v>426.8044581191411</v>
       </c>
       <c r="H21" t="n">
-        <v>-15.59770402537679</v>
+        <v>19.63452654741664</v>
       </c>
       <c r="I21" t="n">
-        <v>-15.59770402537679</v>
+        <v>19.63452654741664</v>
       </c>
       <c r="J21" t="n">
-        <v>-15.59770402537679</v>
+        <v>19.63452654741664</v>
       </c>
       <c r="K21" t="n">
-        <v>-15.59770402537679</v>
+        <v>19.63452654741664</v>
       </c>
       <c r="L21" t="n">
-        <v>-15.59770402537679</v>
+        <v>19.63452654741664</v>
       </c>
       <c r="M21" t="n">
-        <v>-15.59770402537679</v>
+        <v>19.63452654741664</v>
       </c>
       <c r="N21" t="n">
         <v>0</v>
@@ -1576,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="Q21" t="n">
-        <v>399.9196916190625</v>
+        <v>446.4389846665578</v>
       </c>
     </row>
     <row r="22">
@@ -1584,40 +1584,40 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="n">
-        <v>43344</v>
+        <v>43497</v>
       </c>
       <c r="C22" t="n">
-        <v>417.7264836668182</v>
+        <v>428.5848447619122</v>
       </c>
       <c r="D22" t="n">
-        <v>372.4946097610184</v>
+        <v>401.192518061568</v>
       </c>
       <c r="E22" t="n">
-        <v>420.1880876124937</v>
+        <v>445.9439803008886</v>
       </c>
       <c r="F22" t="n">
-        <v>417.7264836668182</v>
+        <v>428.5848447619122</v>
       </c>
       <c r="G22" t="n">
-        <v>417.7264836668182</v>
+        <v>428.5848447619122</v>
       </c>
       <c r="H22" t="n">
-        <v>-21.22084590553616</v>
+        <v>-4.941160678901002</v>
       </c>
       <c r="I22" t="n">
-        <v>-21.22084590553616</v>
+        <v>-4.941160678901002</v>
       </c>
       <c r="J22" t="n">
-        <v>-21.22084590553616</v>
+        <v>-4.941160678901002</v>
       </c>
       <c r="K22" t="n">
-        <v>-21.22084590553616</v>
+        <v>-4.941160678901002</v>
       </c>
       <c r="L22" t="n">
-        <v>-21.22084590553616</v>
+        <v>-4.941160678901002</v>
       </c>
       <c r="M22" t="n">
-        <v>-21.22084590553616</v>
+        <v>-4.941160678901002</v>
       </c>
       <c r="N22" t="n">
         <v>0</v>
@@ -1629,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="Q22" t="n">
-        <v>396.505637761282</v>
+        <v>423.6436840830112</v>
       </c>
     </row>
     <row r="23">
@@ -1637,40 +1637,40 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="n">
-        <v>43374</v>
+        <v>43525</v>
       </c>
       <c r="C23" t="n">
-        <v>419.8512580134968</v>
+        <v>430.1929359231249</v>
       </c>
       <c r="D23" t="n">
-        <v>395.5889344728133</v>
+        <v>360.5292250167337</v>
       </c>
       <c r="E23" t="n">
-        <v>440.6679883628047</v>
+        <v>405.4964532955769</v>
       </c>
       <c r="F23" t="n">
-        <v>419.8512580134968</v>
+        <v>430.1929359231249</v>
       </c>
       <c r="G23" t="n">
-        <v>419.8512580134968</v>
+        <v>430.1929359231249</v>
       </c>
       <c r="H23" t="n">
-        <v>-1.911118823995505</v>
+        <v>-46.89273439650098</v>
       </c>
       <c r="I23" t="n">
-        <v>-1.911118823995505</v>
+        <v>-46.89273439650098</v>
       </c>
       <c r="J23" t="n">
-        <v>-1.911118823995505</v>
+        <v>-46.89273439650098</v>
       </c>
       <c r="K23" t="n">
-        <v>-1.911118823995505</v>
+        <v>-46.89273439650098</v>
       </c>
       <c r="L23" t="n">
-        <v>-1.911118823995505</v>
+        <v>-46.89273439650098</v>
       </c>
       <c r="M23" t="n">
-        <v>-1.911118823995505</v>
+        <v>-46.89273439650098</v>
       </c>
       <c r="N23" t="n">
         <v>0</v>
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="Q23" t="n">
-        <v>417.9401391895013</v>
+        <v>383.3002015266239</v>
       </c>
     </row>
     <row r="24">
@@ -1690,40 +1690,40 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="n">
-        <v>43405</v>
+        <v>43556</v>
       </c>
       <c r="C24" t="n">
-        <v>422.0468581717314</v>
+        <v>431.9733225575201</v>
       </c>
       <c r="D24" t="n">
-        <v>415.9478026828011</v>
+        <v>407.0680399218508</v>
       </c>
       <c r="E24" t="n">
-        <v>458.6743046553374</v>
+        <v>452.6455070438922</v>
       </c>
       <c r="F24" t="n">
-        <v>422.0468581717314</v>
+        <v>431.9733225575201</v>
       </c>
       <c r="G24" t="n">
-        <v>422.0468581717314</v>
+        <v>431.9733225575201</v>
       </c>
       <c r="H24" t="n">
-        <v>16.39114834199487</v>
+        <v>-2.127749615595027</v>
       </c>
       <c r="I24" t="n">
-        <v>16.39114834199487</v>
+        <v>-2.127749615595027</v>
       </c>
       <c r="J24" t="n">
-        <v>16.39114834199487</v>
+        <v>-2.127749615595027</v>
       </c>
       <c r="K24" t="n">
-        <v>16.39114834199487</v>
+        <v>-2.127749615595027</v>
       </c>
       <c r="L24" t="n">
-        <v>16.39114834199487</v>
+        <v>-2.127749615595027</v>
       </c>
       <c r="M24" t="n">
-        <v>16.39114834199487</v>
+        <v>-2.127749615595027</v>
       </c>
       <c r="N24" t="n">
         <v>0</v>
@@ -1735,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="Q24" t="n">
-        <v>438.4380065137263</v>
+        <v>429.8455729419251</v>
       </c>
     </row>
     <row r="25">
@@ -1743,40 +1743,40 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="n">
-        <v>43435</v>
+        <v>43586</v>
       </c>
       <c r="C25" t="n">
-        <v>424.1656110786783</v>
+        <v>433.6962773649994</v>
       </c>
       <c r="D25" t="n">
-        <v>429.7376314019197</v>
+        <v>403.6421628607291</v>
       </c>
       <c r="E25" t="n">
-        <v>475.0937869218047</v>
+        <v>449.7021784572793</v>
       </c>
       <c r="F25" t="n">
-        <v>424.1656110786783</v>
+        <v>433.6962773649994</v>
       </c>
       <c r="G25" t="n">
-        <v>424.1656110786783</v>
+        <v>433.6962773649994</v>
       </c>
       <c r="H25" t="n">
-        <v>28.77823929127664</v>
+        <v>-8.411541317538827</v>
       </c>
       <c r="I25" t="n">
-        <v>28.77823929127664</v>
+        <v>-8.411541317538827</v>
       </c>
       <c r="J25" t="n">
-        <v>28.77823929127664</v>
+        <v>-8.411541317538827</v>
       </c>
       <c r="K25" t="n">
-        <v>28.77823929127664</v>
+        <v>-8.411541317538827</v>
       </c>
       <c r="L25" t="n">
-        <v>28.77823929127664</v>
+        <v>-8.411541317538827</v>
       </c>
       <c r="M25" t="n">
-        <v>28.77823929127664</v>
+        <v>-8.411541317538827</v>
       </c>
       <c r="N25" t="n">
         <v>0</v>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="Q25" t="n">
-        <v>452.9438503699549</v>
+        <v>425.2847360474606</v>
       </c>
     </row>
     <row r="26">
@@ -1796,40 +1796,40 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="n">
-        <v>43466</v>
+        <v>43617</v>
       </c>
       <c r="C26" t="n">
-        <v>426.3549890825233</v>
+        <v>435.4766639950808</v>
       </c>
       <c r="D26" t="n">
-        <v>420.9327299809578</v>
+        <v>420.075411991635</v>
       </c>
       <c r="E26" t="n">
-        <v>465.088900598805</v>
+        <v>463.771395048328</v>
       </c>
       <c r="F26" t="n">
-        <v>426.3549890825233</v>
+        <v>435.4766639950808</v>
       </c>
       <c r="G26" t="n">
-        <v>426.3549890825233</v>
+        <v>435.4766639950808</v>
       </c>
       <c r="H26" t="n">
-        <v>16.51892606029864</v>
+        <v>6.720568190789567</v>
       </c>
       <c r="I26" t="n">
-        <v>16.51892606029864</v>
+        <v>6.720568190789567</v>
       </c>
       <c r="J26" t="n">
-        <v>16.51892606029864</v>
+        <v>6.720568190789567</v>
       </c>
       <c r="K26" t="n">
-        <v>16.51892606029864</v>
+        <v>6.720568190789567</v>
       </c>
       <c r="L26" t="n">
-        <v>16.51892606029864</v>
+        <v>6.720568190789567</v>
       </c>
       <c r="M26" t="n">
-        <v>16.51892606029864</v>
+        <v>6.720568190789567</v>
       </c>
       <c r="N26" t="n">
         <v>0</v>
@@ -1841,7 +1841,7 @@
         <v>0</v>
       </c>
       <c r="Q26" t="n">
-        <v>442.873915142822</v>
+        <v>442.1972321858703</v>
       </c>
     </row>
     <row r="27">
@@ -1849,40 +1849,40 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="n">
-        <v>43497</v>
+        <v>43647</v>
       </c>
       <c r="C27" t="n">
-        <v>428.5428287740431</v>
+        <v>437.1996187905842</v>
       </c>
       <c r="D27" t="n">
-        <v>396.5521598784204</v>
+        <v>396.0835103774078</v>
       </c>
       <c r="E27" t="n">
-        <v>443.6007864222921</v>
+        <v>441.639948487012</v>
       </c>
       <c r="F27" t="n">
-        <v>428.5428287740431</v>
+        <v>437.1996187905842</v>
       </c>
       <c r="G27" t="n">
-        <v>428.5428287740431</v>
+        <v>437.1996187905842</v>
       </c>
       <c r="H27" t="n">
-        <v>-10.26855982451061</v>
+        <v>-18.69791348955332</v>
       </c>
       <c r="I27" t="n">
-        <v>-10.26855982451061</v>
+        <v>-18.69791348955332</v>
       </c>
       <c r="J27" t="n">
-        <v>-10.26855982451061</v>
+        <v>-18.69791348955332</v>
       </c>
       <c r="K27" t="n">
-        <v>-10.26855982451061</v>
+        <v>-18.69791348955332</v>
       </c>
       <c r="L27" t="n">
-        <v>-10.26855982451061</v>
+        <v>-18.69791348955332</v>
       </c>
       <c r="M27" t="n">
-        <v>-10.26855982451061</v>
+        <v>-18.69791348955332</v>
       </c>
       <c r="N27" t="n">
         <v>0</v>
@@ -1894,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="Q27" t="n">
-        <v>418.2742689495325</v>
+        <v>418.5017053010309</v>
       </c>
     </row>
     <row r="28">
@@ -1902,40 +1902,40 @@
         <v>26</v>
       </c>
       <c r="B28" s="2" t="n">
-        <v>43525</v>
+        <v>43678</v>
       </c>
       <c r="C28" t="n">
-        <v>430.518942043803</v>
+        <v>438.9800054126044</v>
       </c>
       <c r="D28" t="n">
-        <v>356.0349495433011</v>
+        <v>400.9578594906414</v>
       </c>
       <c r="E28" t="n">
-        <v>401.942473529522</v>
+        <v>443.9274176865717</v>
       </c>
       <c r="F28" t="n">
-        <v>430.518942043803</v>
+        <v>438.9800054126044</v>
       </c>
       <c r="G28" t="n">
-        <v>430.518942043803</v>
+        <v>438.9800054126044</v>
       </c>
       <c r="H28" t="n">
-        <v>-51.73126744669801</v>
+        <v>-16.67695032537542</v>
       </c>
       <c r="I28" t="n">
-        <v>-51.73126744669801</v>
+        <v>-16.67695032537542</v>
       </c>
       <c r="J28" t="n">
-        <v>-51.73126744669801</v>
+        <v>-16.67695032537542</v>
       </c>
       <c r="K28" t="n">
-        <v>-51.73126744669801</v>
+        <v>-16.67695032537542</v>
       </c>
       <c r="L28" t="n">
-        <v>-51.73126744669801</v>
+        <v>-16.67695032537542</v>
       </c>
       <c r="M28" t="n">
-        <v>-51.73126744669801</v>
+        <v>-16.67695032537542</v>
       </c>
       <c r="N28" t="n">
         <v>0</v>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="Q28" t="n">
-        <v>378.787674597105</v>
+        <v>422.303055087229</v>
       </c>
     </row>
     <row r="29">
@@ -1955,40 +1955,40 @@
         <v>27</v>
       </c>
       <c r="B29" s="2" t="n">
-        <v>43556</v>
+        <v>43709</v>
       </c>
       <c r="C29" t="n">
-        <v>432.7067807777693</v>
+        <v>440.7603920386333</v>
       </c>
       <c r="D29" t="n">
-        <v>407.4974475681445</v>
+        <v>389.0477164603836</v>
       </c>
       <c r="E29" t="n">
-        <v>450.1035971839724</v>
+        <v>435.1452435380241</v>
       </c>
       <c r="F29" t="n">
-        <v>432.7067807777693</v>
+        <v>440.7603920386333</v>
       </c>
       <c r="G29" t="n">
-        <v>432.7067807777693</v>
+        <v>440.7603920386333</v>
       </c>
       <c r="H29" t="n">
-        <v>-4.17657060926457</v>
+        <v>-28.25185572784272</v>
       </c>
       <c r="I29" t="n">
-        <v>-4.17657060926457</v>
+        <v>-28.25185572784272</v>
       </c>
       <c r="J29" t="n">
-        <v>-4.17657060926457</v>
+        <v>-28.25185572784272</v>
       </c>
       <c r="K29" t="n">
-        <v>-4.17657060926457</v>
+        <v>-28.25185572784272</v>
       </c>
       <c r="L29" t="n">
-        <v>-4.17657060926457</v>
+        <v>-28.25185572784272</v>
       </c>
       <c r="M29" t="n">
-        <v>-4.17657060926457</v>
+        <v>-28.25185572784272</v>
       </c>
       <c r="N29" t="n">
         <v>0</v>
@@ -2000,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="Q29" t="n">
-        <v>428.5302101685047</v>
+        <v>412.5085363107905</v>
       </c>
     </row>
     <row r="30">
@@ -2008,40 +2008,40 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="n">
-        <v>43586</v>
+        <v>43739</v>
       </c>
       <c r="C30" t="n">
-        <v>434.8240440687043</v>
+        <v>442.483346838016</v>
       </c>
       <c r="D30" t="n">
-        <v>412.5030455611394</v>
+        <v>417.4543517401071</v>
       </c>
       <c r="E30" t="n">
-        <v>456.1282034712823</v>
+        <v>460.8889541023715</v>
       </c>
       <c r="F30" t="n">
-        <v>434.8240440687043</v>
+        <v>442.483346838016</v>
       </c>
       <c r="G30" t="n">
-        <v>434.8240440687043</v>
+        <v>442.483346838016</v>
       </c>
       <c r="H30" t="n">
-        <v>-1.57988541594044</v>
+        <v>-3.435861876235116</v>
       </c>
       <c r="I30" t="n">
-        <v>-1.57988541594044</v>
+        <v>-3.435861876235116</v>
       </c>
       <c r="J30" t="n">
-        <v>-1.57988541594044</v>
+        <v>-3.435861876235116</v>
       </c>
       <c r="K30" t="n">
-        <v>-1.57988541594044</v>
+        <v>-3.435861876235116</v>
       </c>
       <c r="L30" t="n">
-        <v>-1.57988541594044</v>
+        <v>-3.435861876235116</v>
       </c>
       <c r="M30" t="n">
-        <v>-1.57988541594044</v>
+        <v>-3.435861876235116</v>
       </c>
       <c r="N30" t="n">
         <v>0</v>
@@ -2053,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="Q30" t="n">
-        <v>433.2441586527639</v>
+        <v>439.0474849617809</v>
       </c>
     </row>
     <row r="31">
@@ -2061,40 +2061,40 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="n">
-        <v>43617</v>
+        <v>43770</v>
       </c>
       <c r="C31" t="n">
-        <v>437.0118824707851</v>
+        <v>444.2637334689303</v>
       </c>
       <c r="D31" t="n">
-        <v>418.9504192821534</v>
+        <v>439.8493124696566</v>
       </c>
       <c r="E31" t="n">
-        <v>465.3192826741691</v>
+        <v>483.8019345481168</v>
       </c>
       <c r="F31" t="n">
-        <v>437.0118824707851</v>
+        <v>444.2637334689303</v>
       </c>
       <c r="G31" t="n">
-        <v>437.0118824707851</v>
+        <v>444.2637334689303</v>
       </c>
       <c r="H31" t="n">
-        <v>4.918407026980037</v>
+        <v>17.6286818064352</v>
       </c>
       <c r="I31" t="n">
-        <v>4.918407026980037</v>
+        <v>17.6286818064352</v>
       </c>
       <c r="J31" t="n">
-        <v>4.918407026980037</v>
+        <v>17.6286818064352</v>
       </c>
       <c r="K31" t="n">
-        <v>4.918407026980037</v>
+        <v>17.6286818064352</v>
       </c>
       <c r="L31" t="n">
-        <v>4.918407026980037</v>
+        <v>17.6286818064352</v>
       </c>
       <c r="M31" t="n">
-        <v>4.918407026980037</v>
+        <v>17.6286818064352</v>
       </c>
       <c r="N31" t="n">
         <v>0</v>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="Q31" t="n">
-        <v>441.9302894977651</v>
+        <v>461.8924152753655</v>
       </c>
     </row>
     <row r="32">
@@ -2114,40 +2114,40 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="n">
-        <v>43647</v>
+        <v>43800</v>
       </c>
       <c r="C32" t="n">
-        <v>439.1291454405406</v>
+        <v>445.986688273041</v>
       </c>
       <c r="D32" t="n">
-        <v>396.3668772980377</v>
+        <v>461.7332750849748</v>
       </c>
       <c r="E32" t="n">
-        <v>441.8734853021536</v>
+        <v>506.8613253374785</v>
       </c>
       <c r="F32" t="n">
-        <v>439.1291454405406</v>
+        <v>445.986688273041</v>
       </c>
       <c r="G32" t="n">
-        <v>439.1291454405406</v>
+        <v>445.986688273041</v>
       </c>
       <c r="H32" t="n">
-        <v>-20.368660366116</v>
+        <v>38.39386186267262</v>
       </c>
       <c r="I32" t="n">
-        <v>-20.368660366116</v>
+        <v>38.39386186267262</v>
       </c>
       <c r="J32" t="n">
-        <v>-20.368660366116</v>
+        <v>38.39386186267262</v>
       </c>
       <c r="K32" t="n">
-        <v>-20.368660366116</v>
+        <v>38.39386186267262</v>
       </c>
       <c r="L32" t="n">
-        <v>-20.368660366116</v>
+        <v>38.39386186267262</v>
       </c>
       <c r="M32" t="n">
-        <v>-20.368660366116</v>
+        <v>38.39386186267262</v>
       </c>
       <c r="N32" t="n">
         <v>0</v>
@@ -2159,7 +2159,7 @@
         <v>0</v>
       </c>
       <c r="Q32" t="n">
-        <v>418.7604850744246</v>
+        <v>484.3805501357136</v>
       </c>
     </row>
     <row r="33">
@@ -2167,40 +2167,40 @@
         <v>31</v>
       </c>
       <c r="B33" s="2" t="n">
-        <v>43678</v>
+        <v>43831</v>
       </c>
       <c r="C33" t="n">
-        <v>441.3169839546399</v>
+        <v>447.7664438944535</v>
       </c>
       <c r="D33" t="n">
-        <v>403.1617495134558</v>
+        <v>447.157687757057</v>
       </c>
       <c r="E33" t="n">
-        <v>447.6835331889213</v>
+        <v>491.5704308355508</v>
       </c>
       <c r="F33" t="n">
-        <v>441.3169839546399</v>
+        <v>447.7664438944535</v>
       </c>
       <c r="G33" t="n">
-        <v>441.3169839546399</v>
+        <v>447.7664438944535</v>
       </c>
       <c r="H33" t="n">
-        <v>-16.31043541066282</v>
+        <v>22.15434752718195</v>
       </c>
       <c r="I33" t="n">
-        <v>-16.31043541066282</v>
+        <v>22.15434752718195</v>
       </c>
       <c r="J33" t="n">
-        <v>-16.31043541066282</v>
+        <v>22.15434752718195</v>
       </c>
       <c r="K33" t="n">
-        <v>-16.31043541066282</v>
+        <v>22.15434752718195</v>
       </c>
       <c r="L33" t="n">
-        <v>-16.31043541066282</v>
+        <v>22.15434752718195</v>
       </c>
       <c r="M33" t="n">
-        <v>-16.31043541066282</v>
+        <v>22.15434752718195</v>
       </c>
       <c r="N33" t="n">
         <v>0</v>
@@ -2212,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>425.0065485439771</v>
+        <v>469.9207914216354</v>
       </c>
     </row>
     <row r="34">
@@ -2220,40 +2220,40 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="n">
-        <v>43709</v>
+        <v>43862</v>
       </c>
       <c r="C34" t="n">
-        <v>443.5048224687392</v>
+        <v>449.5461995158661</v>
       </c>
       <c r="D34" t="n">
-        <v>393.8122619716447</v>
+        <v>421.4606151786921</v>
       </c>
       <c r="E34" t="n">
-        <v>437.2660403034934</v>
+        <v>467.2215599165083</v>
       </c>
       <c r="F34" t="n">
-        <v>443.5048224687392</v>
+        <v>449.5461995158661</v>
       </c>
       <c r="G34" t="n">
-        <v>443.5048224687392</v>
+        <v>449.5461995158661</v>
       </c>
       <c r="H34" t="n">
-        <v>-29.19552248586148</v>
+        <v>-5.55562325663371</v>
       </c>
       <c r="I34" t="n">
-        <v>-29.19552248586148</v>
+        <v>-5.55562325663371</v>
       </c>
       <c r="J34" t="n">
-        <v>-29.19552248586148</v>
+        <v>-5.55562325663371</v>
       </c>
       <c r="K34" t="n">
-        <v>-29.19552248586148</v>
+        <v>-5.55562325663371</v>
       </c>
       <c r="L34" t="n">
-        <v>-29.19552248586148</v>
+        <v>-5.55562325663371</v>
       </c>
       <c r="M34" t="n">
-        <v>-29.19552248586148</v>
+        <v>-5.55562325663371</v>
       </c>
       <c r="N34" t="n">
         <v>0</v>
@@ -2265,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="Q34" t="n">
-        <v>414.3092999828777</v>
+        <v>443.9905762592323</v>
       </c>
     </row>
     <row r="35">
@@ -2273,40 +2273,40 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="n">
-        <v>43739</v>
+        <v>43891</v>
       </c>
       <c r="C35" t="n">
-        <v>445.6220831823099</v>
+        <v>451.2007933239281</v>
       </c>
       <c r="D35" t="n">
-        <v>422.3646388353042</v>
+        <v>439.1371414888916</v>
       </c>
       <c r="E35" t="n">
-        <v>466.5608653061933</v>
+        <v>484.7312188773578</v>
       </c>
       <c r="F35" t="n">
-        <v>445.6220831823099</v>
+        <v>451.2007933239281</v>
       </c>
       <c r="G35" t="n">
-        <v>445.6220831823099</v>
+        <v>451.2007933239281</v>
       </c>
       <c r="H35" t="n">
-        <v>-0.662943842435197</v>
+        <v>11.50214683292928</v>
       </c>
       <c r="I35" t="n">
-        <v>-0.662943842435197</v>
+        <v>11.50214683292928</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.662943842435197</v>
+        <v>11.50214683292928</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.662943842435197</v>
+        <v>11.50214683292928</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.662943842435197</v>
+        <v>11.50214683292928</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.662943842435197</v>
+        <v>11.50214683292928</v>
       </c>
       <c r="N35" t="n">
         <v>0</v>
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="Q35" t="n">
-        <v>444.9591393398747</v>
+        <v>462.7029401568573</v>
       </c>
     </row>
     <row r="36">
@@ -2326,40 +2326,40 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="n">
-        <v>43770</v>
+        <v>43922</v>
       </c>
       <c r="C36" t="n">
-        <v>447.8099192529996</v>
+        <v>452.9694970497875</v>
       </c>
       <c r="D36" t="n">
-        <v>443.2592915449501</v>
+        <v>395.1525523401901</v>
       </c>
       <c r="E36" t="n">
-        <v>487.0250767245766</v>
+        <v>439.4709734281178</v>
       </c>
       <c r="F36" t="n">
-        <v>447.8099192529996</v>
+        <v>452.9694970497875</v>
       </c>
       <c r="G36" t="n">
-        <v>447.8099192529996</v>
+        <v>452.9694970497875</v>
       </c>
       <c r="H36" t="n">
-        <v>16.98632696132258</v>
+        <v>-35.66486091186226</v>
       </c>
       <c r="I36" t="n">
-        <v>16.98632696132258</v>
+        <v>-35.66486091186226</v>
       </c>
       <c r="J36" t="n">
-        <v>16.98632696132258</v>
+        <v>-35.66486091186226</v>
       </c>
       <c r="K36" t="n">
-        <v>16.98632696132258</v>
+        <v>-35.66486091186226</v>
       </c>
       <c r="L36" t="n">
-        <v>16.98632696132258</v>
+        <v>-35.66486091186226</v>
       </c>
       <c r="M36" t="n">
-        <v>16.98632696132258</v>
+        <v>-35.66486091186226</v>
       </c>
       <c r="N36" t="n">
         <v>0</v>
@@ -2371,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="Q36" t="n">
-        <v>464.7962462143222</v>
+        <v>417.3046361379252</v>
       </c>
     </row>
     <row r="37">
@@ -2379,40 +2379,40 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="n">
-        <v>43800</v>
+        <v>43952</v>
       </c>
       <c r="C37" t="n">
-        <v>449.9271764646945</v>
+        <v>454.6786832126988</v>
       </c>
       <c r="D37" t="n">
-        <v>462.7993724063767</v>
+        <v>414.7453144456364</v>
       </c>
       <c r="E37" t="n">
-        <v>507.0293914751259</v>
+        <v>460.386610605641</v>
       </c>
       <c r="F37" t="n">
-        <v>449.9271764646945</v>
+        <v>454.6786832126988</v>
       </c>
       <c r="G37" t="n">
-        <v>449.9271764646945</v>
+        <v>454.6786832126988</v>
       </c>
       <c r="H37" t="n">
-        <v>34.71840067849396</v>
+        <v>-17.50785324822775</v>
       </c>
       <c r="I37" t="n">
-        <v>34.71840067849396</v>
+        <v>-17.50785324822775</v>
       </c>
       <c r="J37" t="n">
-        <v>34.71840067849396</v>
+        <v>-17.50785324822775</v>
       </c>
       <c r="K37" t="n">
-        <v>34.71840067849396</v>
+        <v>-17.50785324822775</v>
       </c>
       <c r="L37" t="n">
-        <v>34.71840067849396</v>
+        <v>-17.50785324822775</v>
       </c>
       <c r="M37" t="n">
-        <v>34.71840067849396</v>
+        <v>-17.50785324822775</v>
       </c>
       <c r="N37" t="n">
         <v>0</v>
@@ -2424,7 +2424,7 @@
         <v>0</v>
       </c>
       <c r="Q37" t="n">
-        <v>484.6455771431885</v>
+        <v>437.1708299644711</v>
       </c>
     </row>
     <row r="38">
@@ -2432,40 +2432,40 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="n">
-        <v>43831</v>
+        <v>43983</v>
       </c>
       <c r="C38" t="n">
-        <v>452.1150089167792</v>
+        <v>456.4448422477072</v>
       </c>
       <c r="D38" t="n">
-        <v>452.7828277939835</v>
+        <v>415.2909326816331</v>
       </c>
       <c r="E38" t="n">
-        <v>499.1639650445074</v>
+        <v>459.5465942936099</v>
       </c>
       <c r="F38" t="n">
-        <v>452.1150089167792</v>
+        <v>456.4448422477072</v>
       </c>
       <c r="G38" t="n">
-        <v>452.1150089167792</v>
+        <v>456.4448422477072</v>
       </c>
       <c r="H38" t="n">
-        <v>22.9805847355312</v>
+        <v>-19.80466680437893</v>
       </c>
       <c r="I38" t="n">
-        <v>22.9805847355312</v>
+        <v>-19.80466680437893</v>
       </c>
       <c r="J38" t="n">
-        <v>22.9805847355312</v>
+        <v>-19.80466680437893</v>
       </c>
       <c r="K38" t="n">
-        <v>22.9805847355312</v>
+        <v>-19.80466680437893</v>
       </c>
       <c r="L38" t="n">
-        <v>22.9805847355312</v>
+        <v>-19.80466680437893</v>
       </c>
       <c r="M38" t="n">
-        <v>22.9805847355312</v>
+        <v>-19.80466680437893</v>
       </c>
       <c r="N38" t="n">
         <v>0</v>
@@ -2477,7 +2477,7 @@
         <v>0</v>
       </c>
       <c r="Q38" t="n">
-        <v>475.0955936523104</v>
+        <v>436.6401754433282</v>
       </c>
     </row>
     <row r="39">
@@ -2485,40 +2485,40 @@
         <v>37</v>
       </c>
       <c r="B39" s="2" t="n">
-        <v>43862</v>
+        <v>44013</v>
       </c>
       <c r="C39" t="n">
-        <v>454.2981665126781</v>
+        <v>458.1459321327975</v>
       </c>
       <c r="D39" t="n">
-        <v>421.7996435812416</v>
+        <v>430.6484849460261</v>
       </c>
       <c r="E39" t="n">
-        <v>465.7485826033945</v>
+        <v>476.082388157576</v>
       </c>
       <c r="F39" t="n">
-        <v>454.2981665126781</v>
+        <v>458.1459321327975</v>
       </c>
       <c r="G39" t="n">
-        <v>454.2981665126781</v>
+        <v>458.1459321327975</v>
       </c>
       <c r="H39" t="n">
-        <v>-10.72233655595258</v>
+        <v>-4.176873891610749</v>
       </c>
       <c r="I39" t="n">
-        <v>-10.72233655595258</v>
+        <v>-4.176873891610749</v>
       </c>
       <c r="J39" t="n">
-        <v>-10.72233655595258</v>
+        <v>-4.176873891610749</v>
       </c>
       <c r="K39" t="n">
-        <v>-10.72233655595258</v>
+        <v>-4.176873891610749</v>
       </c>
       <c r="L39" t="n">
-        <v>-10.72233655595258</v>
+        <v>-4.176873891610749</v>
       </c>
       <c r="M39" t="n">
-        <v>-10.72233655595258</v>
+        <v>-4.176873891610749</v>
       </c>
       <c r="N39" t="n">
         <v>0</v>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="Q39" t="n">
-        <v>443.5758299567255</v>
+        <v>453.9690582411868</v>
       </c>
     </row>
     <row r="40">
@@ -2538,40 +2538,40 @@
         <v>38</v>
       </c>
       <c r="B40" s="2" t="n">
-        <v>43891</v>
+        <v>44044</v>
       </c>
       <c r="C40" t="n">
-        <v>456.3404752314222</v>
+        <v>459.9037250140576</v>
       </c>
       <c r="D40" t="n">
-        <v>439.7422131393096</v>
+        <v>423.5839846058979</v>
       </c>
       <c r="E40" t="n">
-        <v>482.7925029176116</v>
+        <v>467.8019844610177</v>
       </c>
       <c r="F40" t="n">
-        <v>456.3404752314222</v>
+        <v>459.9037250140576</v>
       </c>
       <c r="G40" t="n">
-        <v>456.3404752314222</v>
+        <v>459.9037250140576</v>
       </c>
       <c r="H40" t="n">
-        <v>4.997517143947881</v>
+        <v>-13.38169811707656</v>
       </c>
       <c r="I40" t="n">
-        <v>4.997517143947881</v>
+        <v>-13.38169811707656</v>
       </c>
       <c r="J40" t="n">
-        <v>4.997517143947881</v>
+        <v>-13.38169811707656</v>
       </c>
       <c r="K40" t="n">
-        <v>4.997517143947881</v>
+        <v>-13.38169811707656</v>
       </c>
       <c r="L40" t="n">
-        <v>4.997517143947881</v>
+        <v>-13.38169811707656</v>
       </c>
       <c r="M40" t="n">
-        <v>4.997517143947881</v>
+        <v>-13.38169811707656</v>
       </c>
       <c r="N40" t="n">
         <v>0</v>
@@ -2583,7 +2583,7 @@
         <v>0</v>
       </c>
       <c r="Q40" t="n">
-        <v>461.3379923753701</v>
+        <v>446.5220268969811</v>
       </c>
     </row>
     <row r="41">
@@ -2591,40 +2591,40 @@
         <v>39</v>
       </c>
       <c r="B41" s="2" t="n">
-        <v>43922</v>
+        <v>44075</v>
       </c>
       <c r="C41" t="n">
-        <v>458.5233479982004</v>
+        <v>459.4328297901009</v>
       </c>
       <c r="D41" t="n">
-        <v>404.1032378854364</v>
+        <v>434.4178423231942</v>
       </c>
       <c r="E41" t="n">
-        <v>448.6340342618909</v>
+        <v>479.9214149027554</v>
       </c>
       <c r="F41" t="n">
-        <v>458.5233479982004</v>
+        <v>459.4328297901009</v>
       </c>
       <c r="G41" t="n">
-        <v>458.5233479982004</v>
+        <v>459.4328297901009</v>
       </c>
       <c r="H41" t="n">
-        <v>-32.44346109109681</v>
+        <v>-1.195234353493645</v>
       </c>
       <c r="I41" t="n">
-        <v>-32.44346109109681</v>
+        <v>-1.195234353493645</v>
       </c>
       <c r="J41" t="n">
-        <v>-32.44346109109681</v>
+        <v>-1.195234353493645</v>
       </c>
       <c r="K41" t="n">
-        <v>-32.44346109109681</v>
+        <v>-1.195234353493645</v>
       </c>
       <c r="L41" t="n">
-        <v>-32.44346109109681</v>
+        <v>-1.195234353493645</v>
       </c>
       <c r="M41" t="n">
-        <v>-32.44346109109681</v>
+        <v>-1.195234353493645</v>
       </c>
       <c r="N41" t="n">
         <v>0</v>
@@ -2636,7 +2636,7 @@
         <v>0</v>
       </c>
       <c r="Q41" t="n">
-        <v>426.0798869071036</v>
+        <v>458.2375954366073</v>
       </c>
     </row>
     <row r="42">
@@ -2644,40 +2644,40 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="n">
-        <v>43952</v>
+        <v>44105</v>
       </c>
       <c r="C42" t="n">
-        <v>460.6358055144374</v>
+        <v>458.9764765489638</v>
       </c>
       <c r="D42" t="n">
-        <v>430.7463494689902</v>
+        <v>433.3987258770517</v>
       </c>
       <c r="E42" t="n">
-        <v>474.1891529435393</v>
+        <v>478.3551829619664</v>
       </c>
       <c r="F42" t="n">
-        <v>460.6358055144374</v>
+        <v>458.9764765489638</v>
       </c>
       <c r="G42" t="n">
-        <v>460.6358055144374</v>
+        <v>458.9764765489638</v>
       </c>
       <c r="H42" t="n">
-        <v>-9.277607358430862</v>
+        <v>-2.457285897331245</v>
       </c>
       <c r="I42" t="n">
-        <v>-9.277607358430862</v>
+        <v>-2.457285897331245</v>
       </c>
       <c r="J42" t="n">
-        <v>-9.277607358430862</v>
+        <v>-2.457285897331245</v>
       </c>
       <c r="K42" t="n">
-        <v>-9.277607358430862</v>
+        <v>-2.457285897331245</v>
       </c>
       <c r="L42" t="n">
-        <v>-9.277607358430862</v>
+        <v>-2.457285897331245</v>
       </c>
       <c r="M42" t="n">
-        <v>-9.277607358430862</v>
+        <v>-2.457285897331245</v>
       </c>
       <c r="N42" t="n">
         <v>0</v>
@@ -2689,7 +2689,7 @@
         <v>0</v>
       </c>
       <c r="Q42" t="n">
-        <v>451.3581981560065</v>
+        <v>456.5191906516326</v>
       </c>
     </row>
     <row r="43">
@@ -2697,40 +2697,40 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="n">
-        <v>43983</v>
+        <v>44136</v>
       </c>
       <c r="C43" t="n">
-        <v>460.4363854342936</v>
+        <v>458.5049115331222</v>
       </c>
       <c r="D43" t="n">
-        <v>412.8933806901863</v>
+        <v>447.1692572468285</v>
       </c>
       <c r="E43" t="n">
-        <v>458.609032602772</v>
+        <v>490.2157197427356</v>
       </c>
       <c r="F43" t="n">
-        <v>460.4363854342936</v>
+        <v>458.5049115331222</v>
       </c>
       <c r="G43" t="n">
-        <v>460.4363854342936</v>
+        <v>458.5049115331222</v>
       </c>
       <c r="H43" t="n">
-        <v>-24.82772621355193</v>
+        <v>9.948567625633935</v>
       </c>
       <c r="I43" t="n">
-        <v>-24.82772621355193</v>
+        <v>9.948567625633935</v>
       </c>
       <c r="J43" t="n">
-        <v>-24.82772621355193</v>
+        <v>9.948567625633935</v>
       </c>
       <c r="K43" t="n">
-        <v>-24.82772621355193</v>
+        <v>9.948567625633935</v>
       </c>
       <c r="L43" t="n">
-        <v>-24.82772621355193</v>
+        <v>9.948567625633935</v>
       </c>
       <c r="M43" t="n">
-        <v>-24.82772621355193</v>
+        <v>9.948567625633935</v>
       </c>
       <c r="N43" t="n">
         <v>0</v>
@@ -2742,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="Q43" t="n">
-        <v>435.6086592207416</v>
+        <v>468.4534791587561</v>
       </c>
     </row>
     <row r="44">
@@ -2750,40 +2750,40 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="n">
-        <v>44013</v>
+        <v>44166</v>
       </c>
       <c r="C44" t="n">
-        <v>460.2433982599609</v>
+        <v>458.0447936622968</v>
       </c>
       <c r="D44" t="n">
-        <v>434.6425640292623</v>
+        <v>446.4232988705225</v>
       </c>
       <c r="E44" t="n">
-        <v>478.4888130670903</v>
+        <v>491.0043548692323</v>
       </c>
       <c r="F44" t="n">
-        <v>460.2433982599609</v>
+        <v>458.0447936622968</v>
       </c>
       <c r="G44" t="n">
-        <v>460.2433982599609</v>
+        <v>458.0447936622968</v>
       </c>
       <c r="H44" t="n">
-        <v>-2.906302212562663</v>
+        <v>11.02819077100643</v>
       </c>
       <c r="I44" t="n">
-        <v>-2.906302212562663</v>
+        <v>11.02819077100643</v>
       </c>
       <c r="J44" t="n">
-        <v>-2.906302212562663</v>
+        <v>11.02819077100643</v>
       </c>
       <c r="K44" t="n">
-        <v>-2.906302212562663</v>
+        <v>11.02819077100643</v>
       </c>
       <c r="L44" t="n">
-        <v>-2.906302212562663</v>
+        <v>11.02819077100643</v>
       </c>
       <c r="M44" t="n">
-        <v>-2.906302212562663</v>
+        <v>11.02819077100643</v>
       </c>
       <c r="N44" t="n">
         <v>0</v>
@@ -2795,7 +2795,7 @@
         <v>0</v>
       </c>
       <c r="Q44" t="n">
-        <v>457.3370960473982</v>
+        <v>469.0729844333032</v>
       </c>
     </row>
     <row r="45">
@@ -2803,40 +2803,40 @@
         <v>43</v>
       </c>
       <c r="B45" s="2" t="n">
-        <v>44044</v>
+        <v>44197</v>
       </c>
       <c r="C45" t="n">
-        <v>460.0398736525498</v>
+        <v>457.5693385291106</v>
       </c>
       <c r="D45" t="n">
-        <v>422.6116351542519</v>
+        <v>447.9731891826996</v>
       </c>
       <c r="E45" t="n">
-        <v>468.1846690089421</v>
+        <v>494.0605275031571</v>
       </c>
       <c r="F45" t="n">
-        <v>460.0398736525498</v>
+        <v>457.5693385291106</v>
       </c>
       <c r="G45" t="n">
-        <v>460.0398736525498</v>
+        <v>457.5693385291106</v>
       </c>
       <c r="H45" t="n">
-        <v>-14.43954420340467</v>
+        <v>13.8260086013303</v>
       </c>
       <c r="I45" t="n">
-        <v>-14.43954420340467</v>
+        <v>13.8260086013303</v>
       </c>
       <c r="J45" t="n">
-        <v>-14.43954420340467</v>
+        <v>13.8260086013303</v>
       </c>
       <c r="K45" t="n">
-        <v>-14.43954420340467</v>
+        <v>13.8260086013303</v>
       </c>
       <c r="L45" t="n">
-        <v>-14.43954420340467</v>
+        <v>13.8260086013303</v>
       </c>
       <c r="M45" t="n">
-        <v>-14.43954420340467</v>
+        <v>13.8260086013303</v>
       </c>
       <c r="N45" t="n">
         <v>0</v>
@@ -2848,7 +2848,7 @@
         <v>0</v>
       </c>
       <c r="Q45" t="n">
-        <v>445.6003294491451</v>
+        <v>471.3953471304409</v>
       </c>
     </row>
     <row r="46">
@@ -2856,40 +2856,40 @@
         <v>44</v>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44075</v>
+        <v>44228</v>
       </c>
       <c r="C46" t="n">
-        <v>459.8363490451388</v>
+        <v>457.0878465236862</v>
       </c>
       <c r="D46" t="n">
-        <v>431.1788424597819</v>
+        <v>429.0217183535389</v>
       </c>
       <c r="E46" t="n">
-        <v>477.6072426586386</v>
+        <v>476.3931982584392</v>
       </c>
       <c r="F46" t="n">
-        <v>459.8363490451388</v>
+        <v>457.0878465236862</v>
       </c>
       <c r="G46" t="n">
-        <v>459.8363490451388</v>
+        <v>457.0878465236862</v>
       </c>
       <c r="H46" t="n">
-        <v>-5.131253584566888</v>
+        <v>-4.710784620873486</v>
       </c>
       <c r="I46" t="n">
-        <v>-5.131253584566888</v>
+        <v>-4.710784620873486</v>
       </c>
       <c r="J46" t="n">
-        <v>-5.131253584566888</v>
+        <v>-4.710784620873486</v>
       </c>
       <c r="K46" t="n">
-        <v>-5.131253584566888</v>
+        <v>-4.710784620873486</v>
       </c>
       <c r="L46" t="n">
-        <v>-5.131253584566888</v>
+        <v>-4.710784620873486</v>
       </c>
       <c r="M46" t="n">
-        <v>-5.131253584566888</v>
+        <v>-4.710784620873486</v>
       </c>
       <c r="N46" t="n">
         <v>0</v>
@@ -2901,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="Q46" t="n">
-        <v>454.7050954605719</v>
+        <v>452.3770619028127</v>
       </c>
     </row>
     <row r="47">
@@ -2909,40 +2909,40 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="n">
-        <v>44105</v>
+        <v>44256</v>
       </c>
       <c r="C47" t="n">
-        <v>459.6377534564176</v>
+        <v>456.6529505187867</v>
       </c>
       <c r="D47" t="n">
-        <v>432.9246034139124</v>
+        <v>425.4512319630863</v>
       </c>
       <c r="E47" t="n">
-        <v>478.9861434972488</v>
+        <v>470.185811667817</v>
       </c>
       <c r="F47" t="n">
-        <v>459.6377534564176</v>
+        <v>456.6529505187867</v>
       </c>
       <c r="G47" t="n">
-        <v>459.6377534564176</v>
+        <v>456.6529505187867</v>
       </c>
       <c r="H47" t="n">
-        <v>-3.861779259345107</v>
+        <v>-8.197018457645139</v>
       </c>
       <c r="I47" t="n">
-        <v>-3.861779259345107</v>
+        <v>-8.197018457645139</v>
       </c>
       <c r="J47" t="n">
-        <v>-3.861779259345107</v>
+        <v>-8.197018457645139</v>
       </c>
       <c r="K47" t="n">
-        <v>-3.861779259345107</v>
+        <v>-8.197018457645139</v>
       </c>
       <c r="L47" t="n">
-        <v>-3.861779259345107</v>
+        <v>-8.197018457645139</v>
       </c>
       <c r="M47" t="n">
-        <v>-3.861779259345107</v>
+        <v>-8.197018457645139</v>
       </c>
       <c r="N47" t="n">
         <v>0</v>
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="Q47" t="n">
-        <v>455.7759741970725</v>
+        <v>448.4559320611416</v>
       </c>
     </row>
     <row r="48">
@@ -2962,40 +2962,40 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44136</v>
+        <v>44287</v>
       </c>
       <c r="C48" t="n">
-        <v>459.432538014739</v>
+        <v>456.1709448813372</v>
       </c>
       <c r="D48" t="n">
-        <v>451.1854701703989</v>
+        <v>409.4800999884233</v>
       </c>
       <c r="E48" t="n">
-        <v>496.9626861643273</v>
+        <v>452.8972864059012</v>
       </c>
       <c r="F48" t="n">
-        <v>459.432538014739</v>
+        <v>456.1709448813372</v>
       </c>
       <c r="G48" t="n">
-        <v>459.432538014739</v>
+        <v>456.1709448813372</v>
       </c>
       <c r="H48" t="n">
-        <v>15.62716701592273</v>
+        <v>-24.88106629833149</v>
       </c>
       <c r="I48" t="n">
-        <v>15.62716701592273</v>
+        <v>-24.88106629833149</v>
       </c>
       <c r="J48" t="n">
-        <v>15.62716701592273</v>
+        <v>-24.88106629833149</v>
       </c>
       <c r="K48" t="n">
-        <v>15.62716701592273</v>
+        <v>-24.88106629833149</v>
       </c>
       <c r="L48" t="n">
-        <v>15.62716701592273</v>
+        <v>-24.88106629833149</v>
       </c>
       <c r="M48" t="n">
-        <v>15.62716701592273</v>
+        <v>-24.88106629833149</v>
       </c>
       <c r="N48" t="n">
         <v>0</v>
@@ -3007,7 +3007,7 @@
         <v>0</v>
       </c>
       <c r="Q48" t="n">
-        <v>475.0597050306617</v>
+        <v>431.2898785830057</v>
       </c>
     </row>
     <row r="49">
@@ -3015,40 +3015,40 @@
         <v>47</v>
       </c>
       <c r="B49" s="2" t="n">
-        <v>44166</v>
+        <v>44317</v>
       </c>
       <c r="C49" t="n">
-        <v>459.2336025278141</v>
+        <v>455.7044878128377</v>
       </c>
       <c r="D49" t="n">
-        <v>454.6246642200244</v>
+        <v>418.3025697947095</v>
       </c>
       <c r="E49" t="n">
-        <v>498.3411338224678</v>
+        <v>462.2829259548074</v>
       </c>
       <c r="F49" t="n">
-        <v>459.2336025278141</v>
+        <v>455.7044878128377</v>
       </c>
       <c r="G49" t="n">
-        <v>459.2336025278141</v>
+        <v>455.7044878128377</v>
       </c>
       <c r="H49" t="n">
-        <v>17.02425593286465</v>
+        <v>-14.51061499600625</v>
       </c>
       <c r="I49" t="n">
-        <v>17.02425593286465</v>
+        <v>-14.51061499600625</v>
       </c>
       <c r="J49" t="n">
-        <v>17.02425593286465</v>
+        <v>-14.51061499600625</v>
       </c>
       <c r="K49" t="n">
-        <v>17.02425593286465</v>
+        <v>-14.51061499600625</v>
       </c>
       <c r="L49" t="n">
-        <v>17.02425593286465</v>
+        <v>-14.51061499600625</v>
       </c>
       <c r="M49" t="n">
-        <v>17.02425593286465</v>
+        <v>-14.51061499600625</v>
       </c>
       <c r="N49" t="n">
         <v>0</v>
@@ -3060,7 +3060,7 @@
         <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>476.2578584606787</v>
+        <v>441.1938728168314</v>
       </c>
     </row>
     <row r="50">
@@ -3068,40 +3068,40 @@
         <v>48</v>
       </c>
       <c r="B50" s="2" t="n">
-        <v>44197</v>
+        <v>44348</v>
       </c>
       <c r="C50" t="n">
-        <v>459.0280358579917</v>
+        <v>455.222475527031</v>
       </c>
       <c r="D50" t="n">
-        <v>439.3848834222275</v>
+        <v>422.9748759264409</v>
       </c>
       <c r="E50" t="n">
-        <v>484.7044727813781</v>
+        <v>467.3083939585555</v>
       </c>
       <c r="F50" t="n">
-        <v>459.0280358579917</v>
+        <v>455.222475527031</v>
       </c>
       <c r="G50" t="n">
-        <v>459.0280358579917</v>
+        <v>455.222475527031</v>
       </c>
       <c r="H50" t="n">
-        <v>3.015601448872476</v>
+        <v>-10.80953905601923</v>
       </c>
       <c r="I50" t="n">
-        <v>3.015601448872476</v>
+        <v>-10.80953905601923</v>
       </c>
       <c r="J50" t="n">
-        <v>3.015601448872476</v>
+        <v>-10.80953905601923</v>
       </c>
       <c r="K50" t="n">
-        <v>3.015601448872476</v>
+        <v>-10.80953905601923</v>
       </c>
       <c r="L50" t="n">
-        <v>3.015601448872476</v>
+        <v>-10.80953905601923</v>
       </c>
       <c r="M50" t="n">
-        <v>3.015601448872476</v>
+        <v>-10.80953905601923</v>
       </c>
       <c r="N50" t="n">
         <v>0</v>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="Q50" t="n">
-        <v>462.0436373068642</v>
+        <v>444.4129364710118</v>
       </c>
     </row>
     <row r="51">
@@ -3121,40 +3121,40 @@
         <v>49</v>
       </c>
       <c r="B51" s="2" t="n">
-        <v>44228</v>
+        <v>44378</v>
       </c>
       <c r="C51" t="n">
-        <v>458.8200688791777</v>
+        <v>454.7560120246375</v>
       </c>
       <c r="D51" t="n">
-        <v>426.3013509355247</v>
+        <v>423.2415292707394</v>
       </c>
       <c r="E51" t="n">
-        <v>470.6004196626584</v>
+        <v>467.6403497286844</v>
       </c>
       <c r="F51" t="n">
-        <v>458.8200688791777</v>
+        <v>454.7560120246375</v>
       </c>
       <c r="G51" t="n">
-        <v>458.8200688791777</v>
+        <v>454.7560120246375</v>
       </c>
       <c r="H51" t="n">
-        <v>-10.44845217155811</v>
+        <v>-8.794431777408132</v>
       </c>
       <c r="I51" t="n">
-        <v>-10.44845217155811</v>
+        <v>-8.794431777408132</v>
       </c>
       <c r="J51" t="n">
-        <v>-10.44845217155811</v>
+        <v>-8.794431777408132</v>
       </c>
       <c r="K51" t="n">
-        <v>-10.44845217155811</v>
+        <v>-8.794431777408132</v>
       </c>
       <c r="L51" t="n">
-        <v>-10.44845217155811</v>
+        <v>-8.794431777408132</v>
       </c>
       <c r="M51" t="n">
-        <v>-10.44845217155811</v>
+        <v>-8.794431777408132</v>
       </c>
       <c r="N51" t="n">
         <v>0</v>
@@ -3166,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="Q51" t="n">
-        <v>448.3716167076196</v>
+        <v>445.9615802472294</v>
       </c>
     </row>
     <row r="52">
@@ -3174,40 +3174,40 @@
         <v>50</v>
       </c>
       <c r="B52" s="2" t="n">
-        <v>44256</v>
+        <v>44409</v>
       </c>
       <c r="C52" t="n">
-        <v>458.6322277370231</v>
+        <v>454.2739997388309</v>
       </c>
       <c r="D52" t="n">
-        <v>422.9273184111652</v>
+        <v>417.7831690193669</v>
       </c>
       <c r="E52" t="n">
-        <v>465.8027258209181</v>
+        <v>461.2890113124664</v>
       </c>
       <c r="F52" t="n">
-        <v>458.6322277370231</v>
+        <v>454.2739997388309</v>
       </c>
       <c r="G52" t="n">
-        <v>458.6322277370231</v>
+        <v>454.2739997388309</v>
       </c>
       <c r="H52" t="n">
-        <v>-14.10656901539908</v>
+        <v>-14.36160343904983</v>
       </c>
       <c r="I52" t="n">
-        <v>-14.10656901539908</v>
+        <v>-14.36160343904983</v>
       </c>
       <c r="J52" t="n">
-        <v>-14.10656901539908</v>
+        <v>-14.36160343904983</v>
       </c>
       <c r="K52" t="n">
-        <v>-14.10656901539908</v>
+        <v>-14.36160343904983</v>
       </c>
       <c r="L52" t="n">
-        <v>-14.10656901539908</v>
+        <v>-14.36160343904983</v>
       </c>
       <c r="M52" t="n">
-        <v>-14.10656901539908</v>
+        <v>-14.36160343904983</v>
       </c>
       <c r="N52" t="n">
         <v>0</v>
@@ -3219,7 +3219,7 @@
         <v>0</v>
       </c>
       <c r="Q52" t="n">
-        <v>444.525658721624</v>
+        <v>439.9123962997811</v>
       </c>
     </row>
     <row r="53">
@@ -3227,40 +3227,40 @@
         <v>51</v>
       </c>
       <c r="B53" s="2" t="n">
-        <v>44287</v>
+        <v>44440</v>
       </c>
       <c r="C53" t="n">
-        <v>458.4228168667923</v>
+        <v>453.7919874530243</v>
       </c>
       <c r="D53" t="n">
-        <v>414.158814931751</v>
+        <v>420.1295078676861</v>
       </c>
       <c r="E53" t="n">
-        <v>456.9090366595965</v>
+        <v>466.6854541951429</v>
       </c>
       <c r="F53" t="n">
-        <v>458.4228168667923</v>
+        <v>453.7919874530243</v>
       </c>
       <c r="G53" t="n">
-        <v>458.4228168667923</v>
+        <v>453.7919874530243</v>
       </c>
       <c r="H53" t="n">
-        <v>-23.39617043646775</v>
+        <v>-10.25289263087131</v>
       </c>
       <c r="I53" t="n">
-        <v>-23.39617043646775</v>
+        <v>-10.25289263087131</v>
       </c>
       <c r="J53" t="n">
-        <v>-23.39617043646775</v>
+        <v>-10.25289263087131</v>
       </c>
       <c r="K53" t="n">
-        <v>-23.39617043646775</v>
+        <v>-10.25289263087131</v>
       </c>
       <c r="L53" t="n">
-        <v>-23.39617043646775</v>
+        <v>-10.25289263087131</v>
       </c>
       <c r="M53" t="n">
-        <v>-23.39617043646775</v>
+        <v>-10.25289263087131</v>
       </c>
       <c r="N53" t="n">
         <v>0</v>
@@ -3272,7 +3272,7 @@
         <v>0</v>
       </c>
       <c r="Q53" t="n">
-        <v>435.0266464303245</v>
+        <v>443.5390948221529</v>
       </c>
     </row>
     <row r="54">
@@ -3280,40 +3280,40 @@
         <v>52</v>
       </c>
       <c r="B54" s="2" t="n">
-        <v>44317</v>
+        <v>44470</v>
       </c>
       <c r="C54" t="n">
-        <v>458.2201611859237</v>
+        <v>453.3255239506307</v>
       </c>
       <c r="D54" t="n">
-        <v>430.6328492235565</v>
+        <v>428.8577973730919</v>
       </c>
       <c r="E54" t="n">
-        <v>474.6373068842716</v>
+        <v>473.3624923606179</v>
       </c>
       <c r="F54" t="n">
-        <v>458.2201611859237</v>
+        <v>453.3255239506307</v>
       </c>
       <c r="G54" t="n">
-        <v>458.2201611859237</v>
+        <v>453.3255239506307</v>
       </c>
       <c r="H54" t="n">
-        <v>-6.776698958441738</v>
+        <v>-3.024207560279611</v>
       </c>
       <c r="I54" t="n">
-        <v>-6.776698958441738</v>
+        <v>-3.024207560279611</v>
       </c>
       <c r="J54" t="n">
-        <v>-6.776698958441738</v>
+        <v>-3.024207560279611</v>
       </c>
       <c r="K54" t="n">
-        <v>-6.776698958441738</v>
+        <v>-3.024207560279611</v>
       </c>
       <c r="L54" t="n">
-        <v>-6.776698958441738</v>
+        <v>-3.024207560279611</v>
       </c>
       <c r="M54" t="n">
-        <v>-6.776698958441738</v>
+        <v>-3.024207560279611</v>
       </c>
       <c r="N54" t="n">
         <v>0</v>
@@ -3325,7 +3325,7 @@
         <v>0</v>
       </c>
       <c r="Q54" t="n">
-        <v>451.443462227482</v>
+        <v>450.3013163903511</v>
       </c>
     </row>
     <row r="55">
@@ -3333,40 +3333,40 @@
         <v>53</v>
       </c>
       <c r="B55" s="2" t="n">
-        <v>44348</v>
+        <v>44501</v>
       </c>
       <c r="C55" t="n">
-        <v>458.0107503156929</v>
+        <v>452.8435116648241</v>
       </c>
       <c r="D55" t="n">
-        <v>419.4357646557497</v>
+        <v>443.970744197972</v>
       </c>
       <c r="E55" t="n">
-        <v>465.0654045704884</v>
+        <v>487.1439783596479</v>
       </c>
       <c r="F55" t="n">
-        <v>458.0107503156929</v>
+        <v>452.8435116648241</v>
       </c>
       <c r="G55" t="n">
-        <v>458.0107503156929</v>
+        <v>452.8435116648241</v>
       </c>
       <c r="H55" t="n">
-        <v>-14.76870261925649</v>
+        <v>12.3074924475144</v>
       </c>
       <c r="I55" t="n">
-        <v>-14.76870261925649</v>
+        <v>12.3074924475144</v>
       </c>
       <c r="J55" t="n">
-        <v>-14.76870261925649</v>
+        <v>12.3074924475144</v>
       </c>
       <c r="K55" t="n">
-        <v>-14.76870261925649</v>
+        <v>12.3074924475144</v>
       </c>
       <c r="L55" t="n">
-        <v>-14.76870261925649</v>
+        <v>12.3074924475144</v>
       </c>
       <c r="M55" t="n">
-        <v>-14.76870261925649</v>
+        <v>12.3074924475144</v>
       </c>
       <c r="N55" t="n">
         <v>0</v>
@@ -3378,7 +3378,7 @@
         <v>0</v>
       </c>
       <c r="Q55" t="n">
-        <v>443.2420476964364</v>
+        <v>465.1510041123385</v>
       </c>
     </row>
     <row r="56">
@@ -3386,40 +3386,40 @@
         <v>54</v>
       </c>
       <c r="B56" s="2" t="n">
-        <v>44378</v>
+        <v>44531</v>
       </c>
       <c r="C56" t="n">
-        <v>457.8080946348243</v>
+        <v>452.3770481624306</v>
       </c>
       <c r="D56" t="n">
-        <v>427.5751454653267</v>
+        <v>450.1940085153727</v>
       </c>
       <c r="E56" t="n">
-        <v>471.4849898493352</v>
+        <v>494.475595629268</v>
       </c>
       <c r="F56" t="n">
-        <v>457.8080946348243</v>
+        <v>452.3770481624306</v>
       </c>
       <c r="G56" t="n">
-        <v>457.8080946348243</v>
+        <v>452.3770481624306</v>
       </c>
       <c r="H56" t="n">
-        <v>-8.508871626369453</v>
+        <v>20.18722681313517</v>
       </c>
       <c r="I56" t="n">
-        <v>-8.508871626369453</v>
+        <v>20.18722681313517</v>
       </c>
       <c r="J56" t="n">
-        <v>-8.508871626369453</v>
+        <v>20.18722681313517</v>
       </c>
       <c r="K56" t="n">
-        <v>-8.508871626369453</v>
+        <v>20.18722681313517</v>
       </c>
       <c r="L56" t="n">
-        <v>-8.508871626369453</v>
+        <v>20.18722681313517</v>
       </c>
       <c r="M56" t="n">
-        <v>-8.508871626369453</v>
+        <v>20.18722681313517</v>
       </c>
       <c r="N56" t="n">
         <v>0</v>
@@ -3431,7 +3431,7 @@
         <v>0</v>
       </c>
       <c r="Q56" t="n">
-        <v>449.2992230084548</v>
+        <v>472.5642749755658</v>
       </c>
     </row>
     <row r="57">
@@ -3439,40 +3439,40 @@
         <v>55</v>
       </c>
       <c r="B57" s="2" t="n">
-        <v>44409</v>
+        <v>44562</v>
       </c>
       <c r="C57" t="n">
-        <v>457.5986837645935</v>
+        <v>451.895035876624</v>
       </c>
       <c r="D57" t="n">
-        <v>419.2094420669937</v>
+        <v>447.3069391442269</v>
       </c>
       <c r="E57" t="n">
-        <v>464.3195086793157</v>
+        <v>490.405600517599</v>
       </c>
       <c r="F57" t="n">
-        <v>457.5986837645935</v>
+        <v>451.895035876624</v>
       </c>
       <c r="G57" t="n">
-        <v>457.5986837645935</v>
+        <v>451.895035876624</v>
       </c>
       <c r="H57" t="n">
-        <v>-14.97240095257905</v>
+        <v>16.85658590104084</v>
       </c>
       <c r="I57" t="n">
-        <v>-14.97240095257905</v>
+        <v>16.85658590104084</v>
       </c>
       <c r="J57" t="n">
-        <v>-14.97240095257905</v>
+        <v>16.85658590104084</v>
       </c>
       <c r="K57" t="n">
-        <v>-14.97240095257905</v>
+        <v>16.85658590104084</v>
       </c>
       <c r="L57" t="n">
-        <v>-14.97240095257905</v>
+        <v>16.85658590104084</v>
       </c>
       <c r="M57" t="n">
-        <v>-14.97240095257905</v>
+        <v>16.85658590104084</v>
       </c>
       <c r="N57" t="n">
         <v>0</v>
@@ -3484,7 +3484,7 @@
         <v>0</v>
       </c>
       <c r="Q57" t="n">
-        <v>442.6262828120144</v>
+        <v>468.7516217776648</v>
       </c>
     </row>
     <row r="58">
@@ -3492,40 +3492,40 @@
         <v>56</v>
       </c>
       <c r="B58" s="2" t="n">
-        <v>44440</v>
+        <v>44593</v>
       </c>
       <c r="C58" t="n">
-        <v>457.3892728943626</v>
+        <v>451.4130235908174</v>
       </c>
       <c r="D58" t="n">
-        <v>421.175655160299</v>
+        <v>424.4329809342003</v>
       </c>
       <c r="E58" t="n">
-        <v>466.5218719062838</v>
+        <v>468.9002039969044</v>
       </c>
       <c r="F58" t="n">
-        <v>457.3892728943626</v>
+        <v>451.4130235908174</v>
       </c>
       <c r="G58" t="n">
-        <v>457.3892728943626</v>
+        <v>451.4130235908174</v>
       </c>
       <c r="H58" t="n">
-        <v>-13.19604518693713</v>
+        <v>-4.658038358988417</v>
       </c>
       <c r="I58" t="n">
-        <v>-13.19604518693713</v>
+        <v>-4.658038358988417</v>
       </c>
       <c r="J58" t="n">
-        <v>-13.19604518693713</v>
+        <v>-4.658038358988417</v>
       </c>
       <c r="K58" t="n">
-        <v>-13.19604518693713</v>
+        <v>-4.658038358988417</v>
       </c>
       <c r="L58" t="n">
-        <v>-13.19604518693713</v>
+        <v>-4.658038358988417</v>
       </c>
       <c r="M58" t="n">
-        <v>-13.19604518693713</v>
+        <v>-4.658038358988417</v>
       </c>
       <c r="N58" t="n">
         <v>0</v>
@@ -3537,7 +3537,7 @@
         <v>0</v>
       </c>
       <c r="Q58" t="n">
-        <v>444.1932277074255</v>
+        <v>446.754985231829</v>
       </c>
     </row>
     <row r="59">
@@ -3545,40 +3545,40 @@
         <v>57</v>
       </c>
       <c r="B59" s="2" t="n">
-        <v>44470</v>
+        <v>44621</v>
       </c>
       <c r="C59" t="n">
-        <v>457.1866172134941</v>
+        <v>450.9776576552501</v>
       </c>
       <c r="D59" t="n">
-        <v>431.7053785205383</v>
+        <v>400.6694145163828</v>
       </c>
       <c r="E59" t="n">
-        <v>476.4632687843681</v>
+        <v>445.7269920851678</v>
       </c>
       <c r="F59" t="n">
-        <v>457.1866172134941</v>
+        <v>450.9776576552501</v>
       </c>
       <c r="G59" t="n">
-        <v>457.1866172134941</v>
+        <v>450.9776576552501</v>
       </c>
       <c r="H59" t="n">
-        <v>-2.977234654756574</v>
+        <v>-27.66902297302736</v>
       </c>
       <c r="I59" t="n">
-        <v>-2.977234654756574</v>
+        <v>-27.66902297302736</v>
       </c>
       <c r="J59" t="n">
-        <v>-2.977234654756574</v>
+        <v>-27.66902297302736</v>
       </c>
       <c r="K59" t="n">
-        <v>-2.977234654756574</v>
+        <v>-27.66902297302736</v>
       </c>
       <c r="L59" t="n">
-        <v>-2.977234654756574</v>
+        <v>-27.66902297302736</v>
       </c>
       <c r="M59" t="n">
-        <v>-2.977234654756574</v>
+        <v>-27.66902297302736</v>
       </c>
       <c r="N59" t="n">
         <v>0</v>
@@ -3590,7 +3590,7 @@
         <v>0</v>
       </c>
       <c r="Q59" t="n">
-        <v>454.2093825587375</v>
+        <v>423.3086346822227</v>
       </c>
     </row>
     <row r="60">
@@ -3598,40 +3598,40 @@
         <v>58</v>
       </c>
       <c r="B60" s="2" t="n">
-        <v>44501</v>
+        <v>44652</v>
       </c>
       <c r="C60" t="n">
-        <v>456.9772063432632</v>
+        <v>450.4956453694434</v>
       </c>
       <c r="D60" t="n">
-        <v>449.646057103635</v>
+        <v>414.9303965203305</v>
       </c>
       <c r="E60" t="n">
-        <v>494.8926610375772</v>
+        <v>460.7668994385729</v>
       </c>
       <c r="F60" t="n">
-        <v>456.9772063432632</v>
+        <v>450.4956453694434</v>
       </c>
       <c r="G60" t="n">
-        <v>456.9772063432632</v>
+        <v>450.4956453694434</v>
       </c>
       <c r="H60" t="n">
-        <v>15.9371259827358</v>
+        <v>-13.69925229558839</v>
       </c>
       <c r="I60" t="n">
-        <v>15.9371259827358</v>
+        <v>-13.69925229558839</v>
       </c>
       <c r="J60" t="n">
-        <v>15.9371259827358</v>
+        <v>-13.69925229558839</v>
       </c>
       <c r="K60" t="n">
-        <v>15.9371259827358</v>
+        <v>-13.69925229558839</v>
       </c>
       <c r="L60" t="n">
-        <v>15.9371259827358</v>
+        <v>-13.69925229558839</v>
       </c>
       <c r="M60" t="n">
-        <v>15.9371259827358</v>
+        <v>-13.69925229558839</v>
       </c>
       <c r="N60" t="n">
         <v>0</v>
@@ -3643,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="Q60" t="n">
-        <v>472.9143323259989</v>
+        <v>436.796393073855</v>
       </c>
     </row>
     <row r="61">
@@ -3651,40 +3651,40 @@
         <v>59</v>
       </c>
       <c r="B61" s="2" t="n">
-        <v>44531</v>
+        <v>44682</v>
       </c>
       <c r="C61" t="n">
-        <v>456.7745506623946</v>
+        <v>450.0291818670499</v>
       </c>
       <c r="D61" t="n">
-        <v>456.796072746686</v>
+        <v>416.0286163284092</v>
       </c>
       <c r="E61" t="n">
-        <v>501.6742310345127</v>
+        <v>461.435728306004</v>
       </c>
       <c r="F61" t="n">
-        <v>456.7745506623946</v>
+        <v>450.0291818670499</v>
       </c>
       <c r="G61" t="n">
-        <v>456.7745506623946</v>
+        <v>450.0291818670499</v>
       </c>
       <c r="H61" t="n">
-        <v>22.87694430918796</v>
+        <v>-11.47527954769004</v>
       </c>
       <c r="I61" t="n">
-        <v>22.87694430918796</v>
+        <v>-11.47527954769004</v>
       </c>
       <c r="J61" t="n">
-        <v>22.87694430918796</v>
+        <v>-11.47527954769004</v>
       </c>
       <c r="K61" t="n">
-        <v>22.87694430918796</v>
+        <v>-11.47527954769004</v>
       </c>
       <c r="L61" t="n">
-        <v>22.87694430918796</v>
+        <v>-11.47527954769004</v>
       </c>
       <c r="M61" t="n">
-        <v>22.87694430918796</v>
+        <v>-11.47527954769004</v>
       </c>
       <c r="N61" t="n">
         <v>0</v>
@@ -3696,7 +3696,7 @@
         <v>0</v>
       </c>
       <c r="Q61" t="n">
-        <v>479.6514949715826</v>
+        <v>438.5539023193599</v>
       </c>
     </row>
     <row r="62">
@@ -3704,40 +3704,40 @@
         <v>60</v>
       </c>
       <c r="B62" s="2" t="n">
-        <v>44562</v>
+        <v>44713</v>
       </c>
       <c r="C62" t="n">
-        <v>456.5651397921637</v>
+        <v>449.5471695812433</v>
       </c>
       <c r="D62" t="n">
-        <v>444.1685418703975</v>
+        <v>425.9974383330116</v>
       </c>
       <c r="E62" t="n">
-        <v>489.037351232208</v>
+        <v>470.496544626251</v>
       </c>
       <c r="F62" t="n">
-        <v>456.5651397921637</v>
+        <v>449.5231937917669</v>
       </c>
       <c r="G62" t="n">
-        <v>456.5651397921637</v>
+        <v>449.563050873178</v>
       </c>
       <c r="H62" t="n">
-        <v>9.860895339205481</v>
+        <v>-1.96408211761725</v>
       </c>
       <c r="I62" t="n">
-        <v>9.860895339205481</v>
+        <v>-1.96408211761725</v>
       </c>
       <c r="J62" t="n">
-        <v>9.860895339205481</v>
+        <v>-1.96408211761725</v>
       </c>
       <c r="K62" t="n">
-        <v>9.860895339205481</v>
+        <v>-1.96408211761725</v>
       </c>
       <c r="L62" t="n">
-        <v>9.860895339205481</v>
+        <v>-1.96408211761725</v>
       </c>
       <c r="M62" t="n">
-        <v>9.860895339205481</v>
+        <v>-1.96408211761725</v>
       </c>
       <c r="N62" t="n">
         <v>0</v>
@@ -3749,7 +3749,7 @@
         <v>0</v>
       </c>
       <c r="Q62" t="n">
-        <v>466.4260351313692</v>
+        <v>447.583087463626</v>
       </c>
     </row>
     <row r="63">
@@ -3757,40 +3757,40 @@
         <v>61</v>
       </c>
       <c r="B63" s="2" t="n">
-        <v>44593</v>
+        <v>44743</v>
       </c>
       <c r="C63" t="n">
-        <v>456.355728921933</v>
+        <v>449.0807060788498</v>
       </c>
       <c r="D63" t="n">
-        <v>424.8529681396334</v>
+        <v>413.7074951745547</v>
       </c>
       <c r="E63" t="n">
-        <v>468.7480712015249</v>
+        <v>458.5860691847739</v>
       </c>
       <c r="F63" t="n">
-        <v>456.355728921933</v>
+        <v>448.9634064756265</v>
       </c>
       <c r="G63" t="n">
-        <v>456.355728921933</v>
+        <v>449.18162346104</v>
       </c>
       <c r="H63" t="n">
-        <v>-10.17627712673498</v>
+        <v>-13.63613033149267</v>
       </c>
       <c r="I63" t="n">
-        <v>-10.17627712673498</v>
+        <v>-13.63613033149267</v>
       </c>
       <c r="J63" t="n">
-        <v>-10.17627712673498</v>
+        <v>-13.63613033149267</v>
       </c>
       <c r="K63" t="n">
-        <v>-10.17627712673498</v>
+        <v>-13.63613033149267</v>
       </c>
       <c r="L63" t="n">
-        <v>-10.17627712673498</v>
+        <v>-13.63613033149267</v>
       </c>
       <c r="M63" t="n">
-        <v>-10.17627712673498</v>
+        <v>-13.63613033149267</v>
       </c>
       <c r="N63" t="n">
         <v>0</v>
@@ -3802,7 +3802,7 @@
         <v>0</v>
       </c>
       <c r="Q63" t="n">
-        <v>446.179451795198</v>
+        <v>435.4445757473571</v>
       </c>
     </row>
     <row r="64">
@@ -3810,40 +3810,40 @@
         <v>62</v>
       </c>
       <c r="B64" s="2" t="n">
-        <v>44621</v>
+        <v>44774</v>
       </c>
       <c r="C64" t="n">
-        <v>456.1665836197889</v>
+        <v>448.5986937930432</v>
       </c>
       <c r="D64" t="n">
-        <v>400.3620799528401</v>
+        <v>411.0486477484519</v>
       </c>
       <c r="E64" t="n">
-        <v>448.6043963914065</v>
+        <v>454.2721895427016</v>
       </c>
       <c r="F64" t="n">
-        <v>456.1665836197889</v>
+        <v>448.357097213795</v>
       </c>
       <c r="G64" t="n">
-        <v>456.1665836197889</v>
+        <v>448.8258271228696</v>
       </c>
       <c r="H64" t="n">
-        <v>-33.02313200123603</v>
+        <v>-15.46192852777488</v>
       </c>
       <c r="I64" t="n">
-        <v>-33.02313200123603</v>
+        <v>-15.46192852777488</v>
       </c>
       <c r="J64" t="n">
-        <v>-33.02313200123603</v>
+        <v>-15.46192852777488</v>
       </c>
       <c r="K64" t="n">
-        <v>-33.02313200123603</v>
+        <v>-15.46192852777488</v>
       </c>
       <c r="L64" t="n">
-        <v>-33.02313200123603</v>
+        <v>-15.46192852777488</v>
       </c>
       <c r="M64" t="n">
-        <v>-33.02313200123603</v>
+        <v>-15.46192852777488</v>
       </c>
       <c r="N64" t="n">
         <v>0</v>
@@ -3855,7 +3855,7 @@
         <v>0</v>
       </c>
       <c r="Q64" t="n">
-        <v>423.1434516185529</v>
+        <v>433.1367652652683</v>
       </c>
     </row>
     <row r="65">
@@ -3863,40 +3863,40 @@
         <v>63</v>
       </c>
       <c r="B65" s="2" t="n">
-        <v>44652</v>
+        <v>44805</v>
       </c>
       <c r="C65" t="n">
-        <v>455.9571727495581</v>
+        <v>448.1166815072365</v>
       </c>
       <c r="D65" t="n">
-        <v>420.2114470835688</v>
+        <v>408.9375853724227</v>
       </c>
       <c r="E65" t="n">
-        <v>464.5726909496516</v>
+        <v>452.8507394639888</v>
       </c>
       <c r="F65" t="n">
-        <v>455.9571727495581</v>
+        <v>447.7041059854723</v>
       </c>
       <c r="G65" t="n">
-        <v>455.9571727495581</v>
+        <v>448.4871028051434</v>
       </c>
       <c r="H65" t="n">
-        <v>-13.97176645237959</v>
+        <v>-19.27572644506709</v>
       </c>
       <c r="I65" t="n">
-        <v>-13.97176645237959</v>
+        <v>-19.27572644506709</v>
       </c>
       <c r="J65" t="n">
-        <v>-13.97176645237959</v>
+        <v>-19.27572644506709</v>
       </c>
       <c r="K65" t="n">
-        <v>-13.97176645237959</v>
+        <v>-19.27572644506709</v>
       </c>
       <c r="L65" t="n">
-        <v>-13.97176645237959</v>
+        <v>-19.27572644506709</v>
       </c>
       <c r="M65" t="n">
-        <v>-13.97176645237959</v>
+        <v>-19.27572644506709</v>
       </c>
       <c r="N65" t="n">
         <v>0</v>
@@ -3908,7 +3908,7 @@
         <v>0</v>
       </c>
       <c r="Q65" t="n">
-        <v>441.9854062971785</v>
+        <v>428.8409550621694</v>
       </c>
     </row>
     <row r="66">
@@ -3916,40 +3916,40 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="n">
-        <v>44682</v>
+        <v>44835</v>
       </c>
       <c r="C66" t="n">
-        <v>455.7545170686896</v>
+        <v>447.6502180048431</v>
       </c>
       <c r="D66" t="n">
-        <v>428.8253544457389</v>
+        <v>422.0092986236989</v>
       </c>
       <c r="E66" t="n">
-        <v>473.1863499573604</v>
+        <v>466.5542888028829</v>
       </c>
       <c r="F66" t="n">
-        <v>455.7238203157932</v>
+        <v>447.0729181606685</v>
       </c>
       <c r="G66" t="n">
-        <v>455.7745252465548</v>
+        <v>448.1872116278058</v>
       </c>
       <c r="H66" t="n">
-        <v>-4.207841127893348</v>
+        <v>-3.350966490776961</v>
       </c>
       <c r="I66" t="n">
-        <v>-4.207841127893348</v>
+        <v>-3.350966490776961</v>
       </c>
       <c r="J66" t="n">
-        <v>-4.207841127893348</v>
+        <v>-3.350966490776961</v>
       </c>
       <c r="K66" t="n">
-        <v>-4.207841127893348</v>
+        <v>-3.350966490776961</v>
       </c>
       <c r="L66" t="n">
-        <v>-4.207841127893348</v>
+        <v>-3.350966490776961</v>
       </c>
       <c r="M66" t="n">
-        <v>-4.207841127893348</v>
+        <v>-3.350966490776961</v>
       </c>
       <c r="N66" t="n">
         <v>0</v>
@@ -3961,7 +3961,7 @@
         <v>0</v>
       </c>
       <c r="Q66" t="n">
-        <v>451.5466759407962</v>
+        <v>444.2992515140661</v>
       </c>
     </row>
     <row r="67">
@@ -3969,40 +3969,40 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="n">
-        <v>44713</v>
+        <v>44866</v>
       </c>
       <c r="C67" t="n">
-        <v>455.5451061984587</v>
+        <v>447.1682057190364</v>
       </c>
       <c r="D67" t="n">
-        <v>429.0910761134549</v>
+        <v>439.7599894393431</v>
       </c>
       <c r="E67" t="n">
-        <v>472.8105881660915</v>
+        <v>484.5317858010806</v>
       </c>
       <c r="F67" t="n">
-        <v>455.3838898743082</v>
+        <v>446.3995440544778</v>
       </c>
       <c r="G67" t="n">
-        <v>455.6742735541171</v>
+        <v>447.9350863199346</v>
       </c>
       <c r="H67" t="n">
-        <v>-4.849368453467444</v>
+        <v>14.86949953643599</v>
       </c>
       <c r="I67" t="n">
-        <v>-4.849368453467444</v>
+        <v>14.86949953643599</v>
       </c>
       <c r="J67" t="n">
-        <v>-4.849368453467444</v>
+        <v>14.86949953643599</v>
       </c>
       <c r="K67" t="n">
-        <v>-4.849368453467444</v>
+        <v>14.86949953643599</v>
       </c>
       <c r="L67" t="n">
-        <v>-4.849368453467444</v>
+        <v>14.86949953643599</v>
       </c>
       <c r="M67" t="n">
-        <v>-4.849368453467444</v>
+        <v>14.86949953643599</v>
       </c>
       <c r="N67" t="n">
         <v>0</v>
@@ -4014,7 +4014,7 @@
         <v>0</v>
       </c>
       <c r="Q67" t="n">
-        <v>450.6957377449912</v>
+        <v>462.0377052554724</v>
       </c>
     </row>
     <row r="68">
@@ -4022,40 +4022,40 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="n">
-        <v>44743</v>
+        <v>44896</v>
       </c>
       <c r="C68" t="n">
-        <v>455.3424505175901</v>
+        <v>446.7017422166429</v>
       </c>
       <c r="D68" t="n">
-        <v>418.06016118501</v>
+        <v>453.4092620221981</v>
       </c>
       <c r="E68" t="n">
-        <v>464.0635717245058</v>
+        <v>498.7821782666405</v>
       </c>
       <c r="F68" t="n">
-        <v>455.0135853384415</v>
+        <v>445.7284118327478</v>
       </c>
       <c r="G68" t="n">
-        <v>455.630113326874</v>
+        <v>447.6958864902988</v>
       </c>
       <c r="H68" t="n">
-        <v>-14.33122397256681</v>
+        <v>29.31348123825721</v>
       </c>
       <c r="I68" t="n">
-        <v>-14.33122397256681</v>
+        <v>29.31348123825721</v>
       </c>
       <c r="J68" t="n">
-        <v>-14.33122397256681</v>
+        <v>29.31348123825721</v>
       </c>
       <c r="K68" t="n">
-        <v>-14.33122397256681</v>
+        <v>29.31348123825721</v>
       </c>
       <c r="L68" t="n">
-        <v>-14.33122397256681</v>
+        <v>29.31348123825721</v>
       </c>
       <c r="M68" t="n">
-        <v>-14.33122397256681</v>
+        <v>29.31348123825721</v>
       </c>
       <c r="N68" t="n">
         <v>0</v>
@@ -4067,7 +4067,7 @@
         <v>0</v>
       </c>
       <c r="Q68" t="n">
-        <v>441.0112265450232</v>
+        <v>476.0152234549001</v>
       </c>
     </row>
     <row r="69">
@@ -4075,40 +4075,40 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="n">
-        <v>44774</v>
+        <v>44927</v>
       </c>
       <c r="C69" t="n">
-        <v>455.1330396473592</v>
+        <v>446.2197299308363</v>
       </c>
       <c r="D69" t="n">
-        <v>417.0872279189424</v>
+        <v>443.3263692442389</v>
       </c>
       <c r="E69" t="n">
-        <v>461.9873118642111</v>
+        <v>487.6468173944942</v>
       </c>
       <c r="F69" t="n">
-        <v>454.645778938303</v>
+        <v>444.9831828246568</v>
       </c>
       <c r="G69" t="n">
-        <v>455.5789923837901</v>
+        <v>447.4520950678846</v>
       </c>
       <c r="H69" t="n">
-        <v>-15.59770402540576</v>
+        <v>19.63452654739125</v>
       </c>
       <c r="I69" t="n">
-        <v>-15.59770402540576</v>
+        <v>19.63452654739125</v>
       </c>
       <c r="J69" t="n">
-        <v>-15.59770402540576</v>
+        <v>19.63452654739125</v>
       </c>
       <c r="K69" t="n">
-        <v>-15.59770402540576</v>
+        <v>19.63452654739125</v>
       </c>
       <c r="L69" t="n">
-        <v>-15.59770402540576</v>
+        <v>19.63452654739125</v>
       </c>
       <c r="M69" t="n">
-        <v>-15.59770402540576</v>
+        <v>19.63452654739125</v>
       </c>
       <c r="N69" t="n">
         <v>0</v>
@@ -4120,7 +4120,7 @@
         <v>0</v>
       </c>
       <c r="Q69" t="n">
-        <v>439.5353356219534</v>
+        <v>465.8542564782275</v>
       </c>
     </row>
     <row r="70">
@@ -4128,40 +4128,40 @@
         <v>68</v>
       </c>
       <c r="B70" s="2" t="n">
-        <v>44805</v>
+        <v>44958</v>
       </c>
       <c r="C70" t="n">
-        <v>454.9236287771284</v>
+        <v>445.7377176450296</v>
       </c>
       <c r="D70" t="n">
-        <v>410.0623838382451</v>
+        <v>418.2255163063905</v>
       </c>
       <c r="E70" t="n">
-        <v>456.2432652365816</v>
+        <v>461.1896277211871</v>
       </c>
       <c r="F70" t="n">
-        <v>454.2226583031412</v>
+        <v>444.2246309798789</v>
       </c>
       <c r="G70" t="n">
-        <v>455.5647516073104</v>
+        <v>447.2200813212106</v>
       </c>
       <c r="H70" t="n">
-        <v>-21.22084590557021</v>
+        <v>-4.941160678961968</v>
       </c>
       <c r="I70" t="n">
-        <v>-21.22084590557021</v>
+        <v>-4.941160678961968</v>
       </c>
       <c r="J70" t="n">
-        <v>-21.22084590557021</v>
+        <v>-4.941160678961968</v>
       </c>
       <c r="K70" t="n">
-        <v>-21.22084590557021</v>
+        <v>-4.941160678961968</v>
       </c>
       <c r="L70" t="n">
-        <v>-21.22084590557021</v>
+        <v>-4.941160678961968</v>
       </c>
       <c r="M70" t="n">
-        <v>-21.22084590557021</v>
+        <v>-4.941160678961968</v>
       </c>
       <c r="N70" t="n">
         <v>0</v>
@@ -4173,7 +4173,7 @@
         <v>0</v>
       </c>
       <c r="Q70" t="n">
-        <v>433.7027828715582</v>
+        <v>440.7965569660677</v>
       </c>
     </row>
     <row r="71">
@@ -4181,40 +4181,40 @@
         <v>69</v>
       </c>
       <c r="B71" s="2" t="n">
-        <v>44835</v>
+        <v>44986</v>
       </c>
       <c r="C71" t="n">
-        <v>454.7209730962599</v>
+        <v>445.3023517094624</v>
       </c>
       <c r="D71" t="n">
-        <v>429.4200782533776</v>
+        <v>377.1089150134547</v>
       </c>
       <c r="E71" t="n">
-        <v>474.9009012902126</v>
+        <v>421.5653139554556</v>
       </c>
       <c r="F71" t="n">
-        <v>453.7466811672039</v>
+        <v>443.5545999884817</v>
       </c>
       <c r="G71" t="n">
-        <v>455.5789549159654</v>
+        <v>447.0306675799027</v>
       </c>
       <c r="H71" t="n">
-        <v>-1.911118824007317</v>
+        <v>-46.89273439646018</v>
       </c>
       <c r="I71" t="n">
-        <v>-1.911118824007317</v>
+        <v>-46.89273439646018</v>
       </c>
       <c r="J71" t="n">
-        <v>-1.911118824007317</v>
+        <v>-46.89273439646018</v>
       </c>
       <c r="K71" t="n">
-        <v>-1.911118824007317</v>
+        <v>-46.89273439646018</v>
       </c>
       <c r="L71" t="n">
-        <v>-1.911118824007317</v>
+        <v>-46.89273439646018</v>
       </c>
       <c r="M71" t="n">
-        <v>-1.911118824007317</v>
+        <v>-46.89273439646018</v>
       </c>
       <c r="N71" t="n">
         <v>0</v>
@@ -4226,7 +4226,7 @@
         <v>0</v>
       </c>
       <c r="Q71" t="n">
-        <v>452.8098542722526</v>
+        <v>398.4096173130022</v>
       </c>
     </row>
     <row r="72">
@@ -4234,40 +4234,40 @@
         <v>70</v>
       </c>
       <c r="B72" s="2" t="n">
-        <v>44866</v>
+        <v>45017</v>
       </c>
       <c r="C72" t="n">
-        <v>454.511562226029</v>
+        <v>444.8203394236558</v>
       </c>
       <c r="D72" t="n">
-        <v>449.1891796613732</v>
+        <v>419.1899805029494</v>
       </c>
       <c r="E72" t="n">
-        <v>493.8353293553675</v>
+        <v>465.1687092375095</v>
       </c>
       <c r="F72" t="n">
-        <v>453.2367007345671</v>
+        <v>442.7521852472611</v>
       </c>
       <c r="G72" t="n">
-        <v>455.6709394665505</v>
+        <v>446.8750814609451</v>
       </c>
       <c r="H72" t="n">
-        <v>16.391148341967</v>
+        <v>-2.127749615595555</v>
       </c>
       <c r="I72" t="n">
-        <v>16.391148341967</v>
+        <v>-2.127749615595555</v>
       </c>
       <c r="J72" t="n">
-        <v>16.391148341967</v>
+        <v>-2.127749615595555</v>
       </c>
       <c r="K72" t="n">
-        <v>16.391148341967</v>
+        <v>-2.127749615595555</v>
       </c>
       <c r="L72" t="n">
-        <v>16.391148341967</v>
+        <v>-2.127749615595555</v>
       </c>
       <c r="M72" t="n">
-        <v>16.391148341967</v>
+        <v>-2.127749615595555</v>
       </c>
       <c r="N72" t="n">
         <v>0</v>
@@ -4279,7 +4279,7 @@
         <v>0</v>
       </c>
       <c r="Q72" t="n">
-        <v>470.902710567996</v>
+        <v>442.6925898080602</v>
       </c>
     </row>
     <row r="73">
@@ -4287,40 +4287,40 @@
         <v>71</v>
       </c>
       <c r="B73" s="2" t="n">
-        <v>44896</v>
+        <v>45047</v>
       </c>
       <c r="C73" t="n">
-        <v>454.3089065451604</v>
+        <v>444.3538759212623</v>
       </c>
       <c r="D73" t="n">
-        <v>460.7905275050109</v>
+        <v>413.4134916496306</v>
       </c>
       <c r="E73" t="n">
-        <v>505.6618264935747</v>
+        <v>458.2316949788856</v>
       </c>
       <c r="F73" t="n">
-        <v>452.7143338202711</v>
+        <v>441.9755575401835</v>
       </c>
       <c r="G73" t="n">
-        <v>455.7523082261688</v>
+        <v>446.7097375709729</v>
       </c>
       <c r="H73" t="n">
-        <v>28.77823929128474</v>
+        <v>-8.411541317552835</v>
       </c>
       <c r="I73" t="n">
-        <v>28.77823929128474</v>
+        <v>-8.411541317552835</v>
       </c>
       <c r="J73" t="n">
-        <v>28.77823929128474</v>
+        <v>-8.411541317552835</v>
       </c>
       <c r="K73" t="n">
-        <v>28.77823929128474</v>
+        <v>-8.411541317552835</v>
       </c>
       <c r="L73" t="n">
-        <v>28.77823929128474</v>
+        <v>-8.411541317552835</v>
       </c>
       <c r="M73" t="n">
-        <v>28.77823929128474</v>
+        <v>-8.411541317552835</v>
       </c>
       <c r="N73" t="n">
         <v>0</v>
@@ -4332,7 +4332,7 @@
         <v>0</v>
       </c>
       <c r="Q73" t="n">
-        <v>483.0871458364452</v>
+        <v>435.9423346037094</v>
       </c>
     </row>
     <row r="74">
@@ -4340,40 +4340,40 @@
         <v>72</v>
       </c>
       <c r="B74" s="2" t="n">
-        <v>44927</v>
+        <v>45078</v>
       </c>
       <c r="C74" t="n">
-        <v>454.0994956749296</v>
+        <v>443.8718636354556</v>
       </c>
       <c r="D74" t="n">
-        <v>448.138977331724</v>
+        <v>426.5249218831512</v>
       </c>
       <c r="E74" t="n">
-        <v>493.3094053572602</v>
+        <v>472.5817311089736</v>
       </c>
       <c r="F74" t="n">
-        <v>452.2132358442268</v>
+        <v>441.2171991326297</v>
       </c>
       <c r="G74" t="n">
-        <v>455.9041532130101</v>
+        <v>446.5905414194823</v>
       </c>
       <c r="H74" t="n">
-        <v>16.51892606027099</v>
+        <v>6.72056819085106</v>
       </c>
       <c r="I74" t="n">
-        <v>16.51892606027099</v>
+        <v>6.72056819085106</v>
       </c>
       <c r="J74" t="n">
-        <v>16.51892606027099</v>
+        <v>6.72056819085106</v>
       </c>
       <c r="K74" t="n">
-        <v>16.51892606027099</v>
+        <v>6.72056819085106</v>
       </c>
       <c r="L74" t="n">
-        <v>16.51892606027099</v>
+        <v>6.72056819085106</v>
       </c>
       <c r="M74" t="n">
-        <v>16.51892606027099</v>
+        <v>6.72056819085106</v>
       </c>
       <c r="N74" t="n">
         <v>0</v>
@@ -4385,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="Q74" t="n">
-        <v>470.6184217352006</v>
+        <v>450.5924318263067</v>
       </c>
     </row>
     <row r="75">
@@ -4393,40 +4393,40 @@
         <v>73</v>
       </c>
       <c r="B75" s="2" t="n">
-        <v>44958</v>
+        <v>45108</v>
       </c>
       <c r="C75" t="n">
-        <v>453.8900848046987</v>
+        <v>443.4054001330621</v>
       </c>
       <c r="D75" t="n">
-        <v>422.3261558375858</v>
+        <v>403.3551482943583</v>
       </c>
       <c r="E75" t="n">
-        <v>465.0719596910144</v>
+        <v>445.1446048764982</v>
       </c>
       <c r="F75" t="n">
-        <v>451.6764080894762</v>
+        <v>440.4378445159048</v>
       </c>
       <c r="G75" t="n">
-        <v>455.9880841811718</v>
+        <v>446.3921509613517</v>
       </c>
       <c r="H75" t="n">
-        <v>-10.26855982453944</v>
+        <v>-18.6979134895627</v>
       </c>
       <c r="I75" t="n">
-        <v>-10.26855982453944</v>
+        <v>-18.6979134895627</v>
       </c>
       <c r="J75" t="n">
-        <v>-10.26855982453944</v>
+        <v>-18.6979134895627</v>
       </c>
       <c r="K75" t="n">
-        <v>-10.26855982453944</v>
+        <v>-18.6979134895627</v>
       </c>
       <c r="L75" t="n">
-        <v>-10.26855982453944</v>
+        <v>-18.6979134895627</v>
       </c>
       <c r="M75" t="n">
-        <v>-10.26855982453944</v>
+        <v>-18.6979134895627</v>
       </c>
       <c r="N75" t="n">
         <v>0</v>
@@ -4438,7 +4438,7 @@
         <v>0</v>
       </c>
       <c r="Q75" t="n">
-        <v>443.6215249801592</v>
+        <v>424.7074866434994</v>
       </c>
     </row>
     <row r="76">
@@ -4446,40 +4446,40 @@
         <v>74</v>
       </c>
       <c r="B76" s="2" t="n">
-        <v>44986</v>
+        <v>45139</v>
       </c>
       <c r="C76" t="n">
-        <v>453.7009395025547</v>
+        <v>442.9233878472555</v>
       </c>
       <c r="D76" t="n">
-        <v>379.382030183885</v>
+        <v>404.3197394418049</v>
       </c>
       <c r="E76" t="n">
-        <v>423.877737233615</v>
+        <v>449.9297825428094</v>
       </c>
       <c r="F76" t="n">
-        <v>451.1584154385191</v>
+        <v>439.5717578165355</v>
       </c>
       <c r="G76" t="n">
-        <v>456.140492125335</v>
+        <v>446.3193860789826</v>
       </c>
       <c r="H76" t="n">
-        <v>-51.7312674466584</v>
+        <v>-16.67695032541693</v>
       </c>
       <c r="I76" t="n">
-        <v>-51.7312674466584</v>
+        <v>-16.67695032541693</v>
       </c>
       <c r="J76" t="n">
-        <v>-51.7312674466584</v>
+        <v>-16.67695032541693</v>
       </c>
       <c r="K76" t="n">
-        <v>-51.7312674466584</v>
+        <v>-16.67695032541693</v>
       </c>
       <c r="L76" t="n">
-        <v>-51.7312674466584</v>
+        <v>-16.67695032541693</v>
       </c>
       <c r="M76" t="n">
-        <v>-51.7312674466584</v>
+        <v>-16.67695032541693</v>
       </c>
       <c r="N76" t="n">
         <v>0</v>
@@ -4491,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="Q76" t="n">
-        <v>401.9696720558963</v>
+        <v>426.2464375218385</v>
       </c>
     </row>
     <row r="77">
@@ -4499,40 +4499,40 @@
         <v>75</v>
       </c>
       <c r="B77" s="2" t="n">
-        <v>45017</v>
+        <v>45170</v>
       </c>
       <c r="C77" t="n">
-        <v>453.4915286323239</v>
+        <v>442.4413755614488</v>
       </c>
       <c r="D77" t="n">
-        <v>426.3957876248249</v>
+        <v>391.3420506655801</v>
       </c>
       <c r="E77" t="n">
-        <v>471.1171329903435</v>
+        <v>435.2239913312363</v>
       </c>
       <c r="F77" t="n">
-        <v>450.6195655631668</v>
+        <v>438.6939770287168</v>
       </c>
       <c r="G77" t="n">
-        <v>456.3745593648537</v>
+        <v>446.1746606607249</v>
       </c>
       <c r="H77" t="n">
-        <v>-4.176570609256751</v>
+        <v>-28.25185572773727</v>
       </c>
       <c r="I77" t="n">
-        <v>-4.176570609256751</v>
+        <v>-28.25185572773727</v>
       </c>
       <c r="J77" t="n">
-        <v>-4.176570609256751</v>
+        <v>-28.25185572773727</v>
       </c>
       <c r="K77" t="n">
-        <v>-4.176570609256751</v>
+        <v>-28.25185572773727</v>
       </c>
       <c r="L77" t="n">
-        <v>-4.176570609256751</v>
+        <v>-28.25185572773727</v>
       </c>
       <c r="M77" t="n">
-        <v>-4.176570609256751</v>
+        <v>-28.25185572773727</v>
       </c>
       <c r="N77" t="n">
         <v>0</v>
@@ -4544,7 +4544,7 @@
         <v>0</v>
       </c>
       <c r="Q77" t="n">
-        <v>449.3149580230671</v>
+        <v>414.1895198337115</v>
       </c>
     </row>
     <row r="78">
@@ -4552,40 +4552,40 @@
         <v>76</v>
       </c>
       <c r="B78" s="2" t="n">
-        <v>45047</v>
+        <v>45200</v>
       </c>
       <c r="C78" t="n">
-        <v>453.2888729514553</v>
+        <v>441.9749120590554</v>
       </c>
       <c r="D78" t="n">
-        <v>429.6718379507798</v>
+        <v>414.0753581974997</v>
       </c>
       <c r="E78" t="n">
-        <v>476.3185731617942</v>
+        <v>460.2984353608328</v>
       </c>
       <c r="F78" t="n">
-        <v>450.1520849194595</v>
+        <v>437.8150471774659</v>
       </c>
       <c r="G78" t="n">
-        <v>456.5499469574943</v>
+        <v>446.0922165807613</v>
       </c>
       <c r="H78" t="n">
-        <v>-1.579885415971567</v>
+        <v>-3.435861876252266</v>
       </c>
       <c r="I78" t="n">
-        <v>-1.579885415971567</v>
+        <v>-3.435861876252266</v>
       </c>
       <c r="J78" t="n">
-        <v>-1.579885415971567</v>
+        <v>-3.435861876252266</v>
       </c>
       <c r="K78" t="n">
-        <v>-1.579885415971567</v>
+        <v>-3.435861876252266</v>
       </c>
       <c r="L78" t="n">
-        <v>-1.579885415971567</v>
+        <v>-3.435861876252266</v>
       </c>
       <c r="M78" t="n">
-        <v>-1.579885415971567</v>
+        <v>-3.435861876252266</v>
       </c>
       <c r="N78" t="n">
         <v>0</v>
@@ -4597,219 +4597,7 @@
         <v>0</v>
       </c>
       <c r="Q78" t="n">
-        <v>451.7089875354837</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" s="2" t="n">
-        <v>45078</v>
-      </c>
-      <c r="C79" t="n">
-        <v>453.0794620812244</v>
-      </c>
-      <c r="D79" t="n">
-        <v>435.667952735714</v>
-      </c>
-      <c r="E79" t="n">
-        <v>480.6409802425715</v>
-      </c>
-      <c r="F79" t="n">
-        <v>449.4825011569953</v>
-      </c>
-      <c r="G79" t="n">
-        <v>456.7374054240873</v>
-      </c>
-      <c r="H79" t="n">
-        <v>4.918407027043419</v>
-      </c>
-      <c r="I79" t="n">
-        <v>4.918407027043419</v>
-      </c>
-      <c r="J79" t="n">
-        <v>4.918407027043419</v>
-      </c>
-      <c r="K79" t="n">
-        <v>4.918407027043419</v>
-      </c>
-      <c r="L79" t="n">
-        <v>4.918407027043419</v>
-      </c>
-      <c r="M79" t="n">
-        <v>4.918407027043419</v>
-      </c>
-      <c r="N79" t="n">
-        <v>0</v>
-      </c>
-      <c r="O79" t="n">
-        <v>0</v>
-      </c>
-      <c r="P79" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q79" t="n">
-        <v>457.9978691082679</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" s="2" t="n">
-        <v>45108</v>
-      </c>
-      <c r="C80" t="n">
-        <v>452.8768064003559</v>
-      </c>
-      <c r="D80" t="n">
-        <v>409.7988902863147</v>
-      </c>
-      <c r="E80" t="n">
-        <v>454.3129410993427</v>
-      </c>
-      <c r="F80" t="n">
-        <v>448.8939464037774</v>
-      </c>
-      <c r="G80" t="n">
-        <v>456.9749595501776</v>
-      </c>
-      <c r="H80" t="n">
-        <v>-20.36866036612081</v>
-      </c>
-      <c r="I80" t="n">
-        <v>-20.36866036612081</v>
-      </c>
-      <c r="J80" t="n">
-        <v>-20.36866036612081</v>
-      </c>
-      <c r="K80" t="n">
-        <v>-20.36866036612081</v>
-      </c>
-      <c r="L80" t="n">
-        <v>-20.36866036612081</v>
-      </c>
-      <c r="M80" t="n">
-        <v>-20.36866036612081</v>
-      </c>
-      <c r="N80" t="n">
-        <v>0</v>
-      </c>
-      <c r="O80" t="n">
-        <v>0</v>
-      </c>
-      <c r="P80" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q80" t="n">
-        <v>432.5081460342351</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B81" s="2" t="n">
-        <v>45139</v>
-      </c>
-      <c r="C81" t="n">
-        <v>452.667395530125</v>
-      </c>
-      <c r="D81" t="n">
-        <v>414.0033069635632</v>
-      </c>
-      <c r="E81" t="n">
-        <v>460.5426526292821</v>
-      </c>
-      <c r="F81" t="n">
-        <v>448.2405433230658</v>
-      </c>
-      <c r="G81" t="n">
-        <v>457.1784210686702</v>
-      </c>
-      <c r="H81" t="n">
-        <v>-16.31043541069441</v>
-      </c>
-      <c r="I81" t="n">
-        <v>-16.31043541069441</v>
-      </c>
-      <c r="J81" t="n">
-        <v>-16.31043541069441</v>
-      </c>
-      <c r="K81" t="n">
-        <v>-16.31043541069441</v>
-      </c>
-      <c r="L81" t="n">
-        <v>-16.31043541069441</v>
-      </c>
-      <c r="M81" t="n">
-        <v>-16.31043541069441</v>
-      </c>
-      <c r="N81" t="n">
-        <v>0</v>
-      </c>
-      <c r="O81" t="n">
-        <v>0</v>
-      </c>
-      <c r="P81" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q81" t="n">
-        <v>436.3569601194306</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="B82" s="2" t="n">
-        <v>45170</v>
-      </c>
-      <c r="C82" t="n">
-        <v>452.4579846598942</v>
-      </c>
-      <c r="D82" t="n">
-        <v>401.0536688318069</v>
-      </c>
-      <c r="E82" t="n">
-        <v>447.5337914048855</v>
-      </c>
-      <c r="F82" t="n">
-        <v>447.6068635134412</v>
-      </c>
-      <c r="G82" t="n">
-        <v>457.4895488066387</v>
-      </c>
-      <c r="H82" t="n">
-        <v>-29.19552248576464</v>
-      </c>
-      <c r="I82" t="n">
-        <v>-29.19552248576464</v>
-      </c>
-      <c r="J82" t="n">
-        <v>-29.19552248576464</v>
-      </c>
-      <c r="K82" t="n">
-        <v>-29.19552248576464</v>
-      </c>
-      <c r="L82" t="n">
-        <v>-29.19552248576464</v>
-      </c>
-      <c r="M82" t="n">
-        <v>-29.19552248576464</v>
-      </c>
-      <c r="N82" t="n">
-        <v>0</v>
-      </c>
-      <c r="O82" t="n">
-        <v>0</v>
-      </c>
-      <c r="P82" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q82" t="n">
-        <v>423.2624621741296</v>
+        <v>438.5390501828031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>